<commit_message>
Fix the data format issue and filled up a blank column in spreadsheet
20726 - Upload data fix
</commit_message>
<xml_diff>
--- a/src/main/resources/OCP.xlsx
+++ b/src/main/resources/OCP.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\c2s-ws\ocp-ws\ocp-test-data\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8895" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8895" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Organizations" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4920" uniqueCount="1908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4921" uniqueCount="1908">
   <si>
     <t>First Name</t>
   </si>
@@ -5793,10 +5793,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="[$-14009]yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="167" formatCode="h:mm;@"/>
-    <numFmt numFmtId="168" formatCode="00000"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-14009]yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="h:mm;@"/>
+    <numFmt numFmtId="167" formatCode="00000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -5991,7 +5991,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6108,14 +6108,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6131,9 +6131,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -6143,14 +6140,20 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -6160,6 +6163,321 @@
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="26">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="00000"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -6193,6 +6511,64 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="double">
+          <color rgb="FF3F3F3F"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color rgb="FF3F3F3F"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14999847407452621"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -6520,379 +6896,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="00000"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="double">
-          <color rgb="FF3F3F3F"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color rgb="FF3F3F3F"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14999847407452621"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="double">
           <color rgb="FF3F3F3F"/>
@@ -6954,33 +6957,33 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I20" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" headerRowCellStyle="Check Cell">
   <autoFilter ref="A1:I20"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="ORGANIZATIONS" dataDxfId="9"/>
-    <tableColumn id="10" name="Location" dataDxfId="8"/>
-    <tableColumn id="6" name="Street" dataDxfId="7"/>
-    <tableColumn id="7" name="City" dataDxfId="6"/>
-    <tableColumn id="8" name="State" dataDxfId="5"/>
-    <tableColumn id="9" name="Zip Code" dataDxfId="4"/>
-    <tableColumn id="3" name="CONTACT" dataDxfId="3"/>
-    <tableColumn id="4" name="IDENTIFIER (ORG TAX ID)" dataDxfId="2"/>
-    <tableColumn id="5" name="STATUS" dataDxfId="1"/>
+    <tableColumn id="1" name="ORGANIZATIONS" dataDxfId="22"/>
+    <tableColumn id="10" name="Location" dataDxfId="21"/>
+    <tableColumn id="6" name="Street" dataDxfId="20"/>
+    <tableColumn id="7" name="City" dataDxfId="19"/>
+    <tableColumn id="8" name="State" dataDxfId="18"/>
+    <tableColumn id="9" name="Zip Code" dataDxfId="17"/>
+    <tableColumn id="3" name="CONTACT" dataDxfId="16"/>
+    <tableColumn id="4" name="IDENTIFIER (ORG TAX ID)" dataDxfId="15"/>
+    <tableColumn id="5" name="STATUS" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:J16" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:J16" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" headerRowCellStyle="Check Cell">
   <tableColumns count="10">
-    <tableColumn id="1" name="Organization" dataDxfId="0"/>
-    <tableColumn id="10" name="Location" dataDxfId="18"/>
-    <tableColumn id="11" name="Street" dataDxfId="17"/>
-    <tableColumn id="9" name="City" dataDxfId="16"/>
-    <tableColumn id="6" name="State" dataDxfId="15"/>
-    <tableColumn id="8" name="Zip Code" dataDxfId="14"/>
-    <tableColumn id="3" name="Contact" dataDxfId="13"/>
-    <tableColumn id="7" name="Identifier Type" dataDxfId="12"/>
-    <tableColumn id="4" name="Identifier" dataDxfId="11"/>
-    <tableColumn id="5" name="STATUS" dataDxfId="10"/>
+    <tableColumn id="1" name="Organization" dataDxfId="9"/>
+    <tableColumn id="10" name="Location" dataDxfId="8"/>
+    <tableColumn id="11" name="Street" dataDxfId="7"/>
+    <tableColumn id="9" name="City" dataDxfId="6"/>
+    <tableColumn id="6" name="State" dataDxfId="5"/>
+    <tableColumn id="8" name="Zip Code" dataDxfId="4"/>
+    <tableColumn id="3" name="Contact" dataDxfId="3"/>
+    <tableColumn id="7" name="Identifier Type" dataDxfId="2"/>
+    <tableColumn id="4" name="Identifier" dataDxfId="1"/>
+    <tableColumn id="5" name="STATUS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8335,41 +8338,41 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="69" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="69" t="s">
+    <row r="13" spans="1:12" s="68" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="68" t="s">
         <v>332</v>
       </c>
-      <c r="C13" s="70" t="s">
+      <c r="C13" s="69" t="s">
         <v>440</v>
       </c>
-      <c r="D13" s="69" t="s">
+      <c r="D13" s="68" t="s">
         <v>298</v>
       </c>
-      <c r="E13" s="69" t="s">
+      <c r="E13" s="68" t="s">
         <v>1418</v>
       </c>
-      <c r="F13" s="69" t="s">
+      <c r="F13" s="68" t="s">
         <v>324</v>
       </c>
-      <c r="G13" s="69" t="s">
+      <c r="G13" s="68" t="s">
         <v>269</v>
       </c>
-      <c r="H13" s="71" t="s">
+      <c r="H13" s="70" t="s">
         <v>1511</v>
       </c>
-      <c r="I13" s="69" t="s">
+      <c r="I13" s="68" t="s">
         <v>325</v>
       </c>
-      <c r="J13" s="72">
+      <c r="J13" s="71">
         <v>43621</v>
       </c>
-      <c r="K13" s="72">
+      <c r="K13" s="71">
         <v>43562</v>
       </c>
-      <c r="L13" s="69" t="s">
+      <c r="L13" s="68" t="s">
         <v>1511</v>
       </c>
     </row>
@@ -9861,7 +9864,7 @@
       <c r="E2" s="36" t="s">
         <v>1519</v>
       </c>
-      <c r="F2" s="73">
+      <c r="F2" s="72">
         <v>20707</v>
       </c>
       <c r="G2" s="35" t="s">
@@ -9893,7 +9896,7 @@
       <c r="E3" s="36" t="s">
         <v>1555</v>
       </c>
-      <c r="F3" s="73">
+      <c r="F3" s="72">
         <v>30513</v>
       </c>
       <c r="G3" s="35" t="s">
@@ -9925,7 +9928,7 @@
       <c r="E4" s="36" t="s">
         <v>1555</v>
       </c>
-      <c r="F4" s="73">
+      <c r="F4" s="72">
         <v>78209</v>
       </c>
       <c r="G4" s="35" t="s">
@@ -9957,7 +9960,7 @@
       <c r="E5" s="36" t="s">
         <v>1558</v>
       </c>
-      <c r="F5" s="73">
+      <c r="F5" s="72">
         <v>11418</v>
       </c>
       <c r="G5" s="35" t="s">
@@ -9989,7 +9992,7 @@
       <c r="E6" s="36" t="s">
         <v>1561</v>
       </c>
-      <c r="F6" s="73">
+      <c r="F6" s="72">
         <v>44128</v>
       </c>
       <c r="G6" s="35" t="s">
@@ -10021,7 +10024,7 @@
       <c r="E7" s="48" t="s">
         <v>1530</v>
       </c>
-      <c r="F7" s="74">
+      <c r="F7" s="73">
         <v>38110</v>
       </c>
       <c r="G7" s="30" t="s">
@@ -10053,7 +10056,7 @@
       <c r="E8" s="48" t="s">
         <v>1564</v>
       </c>
-      <c r="F8" s="74">
+      <c r="F8" s="73">
         <v>32904</v>
       </c>
       <c r="G8" s="30" t="s">
@@ -10085,7 +10088,7 @@
       <c r="E9" s="48" t="s">
         <v>1519</v>
       </c>
-      <c r="F9" s="74">
+      <c r="F9" s="73">
         <v>20815</v>
       </c>
       <c r="G9" s="30" t="s">
@@ -10117,7 +10120,7 @@
       <c r="E10" s="48" t="s">
         <v>1567</v>
       </c>
-      <c r="F10" s="74">
+      <c r="F10" s="73">
         <v>6074</v>
       </c>
       <c r="G10" s="30" t="s">
@@ -10149,7 +10152,7 @@
       <c r="E11" s="48" t="s">
         <v>1530</v>
       </c>
-      <c r="F11" s="74">
+      <c r="F11" s="73">
         <v>96815</v>
       </c>
       <c r="G11" s="30" t="s">
@@ -10181,7 +10184,7 @@
       <c r="E12" s="36" t="s">
         <v>1530</v>
       </c>
-      <c r="F12" s="73">
+      <c r="F12" s="72">
         <v>37216</v>
       </c>
       <c r="G12" s="37" t="s">
@@ -10213,7 +10216,7 @@
       <c r="E13" s="36" t="s">
         <v>1519</v>
       </c>
-      <c r="F13" s="73">
+      <c r="F13" s="72">
         <v>60025</v>
       </c>
       <c r="G13" s="37" t="s">
@@ -10245,7 +10248,7 @@
       <c r="E14" s="36" t="s">
         <v>1555</v>
       </c>
-      <c r="F14" s="73">
+      <c r="F14" s="72">
         <v>56301</v>
       </c>
       <c r="G14" s="37" t="s">
@@ -10277,7 +10280,7 @@
       <c r="E15" s="36" t="s">
         <v>1574</v>
       </c>
-      <c r="F15" s="73">
+      <c r="F15" s="72">
         <v>30269</v>
       </c>
       <c r="G15" s="37" t="s">
@@ -10309,7 +10312,7 @@
       <c r="E16" s="36" t="s">
         <v>1558</v>
       </c>
-      <c r="F16" s="73">
+      <c r="F16" s="72">
         <v>11561</v>
       </c>
       <c r="G16" s="37" t="s">
@@ -10341,7 +10344,7 @@
       <c r="E17" s="48" t="s">
         <v>1519</v>
       </c>
-      <c r="F17" s="74">
+      <c r="F17" s="73">
         <v>21771</v>
       </c>
       <c r="G17" s="28" t="s">
@@ -10373,7 +10376,7 @@
       <c r="E18" s="48" t="s">
         <v>1578</v>
       </c>
-      <c r="F18" s="74">
+      <c r="F18" s="73">
         <v>29708</v>
       </c>
       <c r="G18" s="28" t="s">
@@ -10405,7 +10408,7 @@
       <c r="E19" s="48" t="s">
         <v>1580</v>
       </c>
-      <c r="F19" s="74">
+      <c r="F19" s="73">
         <v>37849</v>
       </c>
       <c r="G19" s="28" t="s">
@@ -10437,7 +10440,7 @@
       <c r="E20" s="48" t="s">
         <v>1530</v>
       </c>
-      <c r="F20" s="74">
+      <c r="F20" s="73">
         <v>23693</v>
       </c>
       <c r="G20" s="28" t="s">
@@ -10469,7 +10472,7 @@
       <c r="E21" s="48" t="s">
         <v>1555</v>
       </c>
-      <c r="F21" s="74">
+      <c r="F21" s="73">
         <v>98512</v>
       </c>
       <c r="G21" s="28" t="s">
@@ -10501,7 +10504,7 @@
       <c r="E22" s="36" t="s">
         <v>1530</v>
       </c>
-      <c r="F22" s="73">
+      <c r="F22" s="72">
         <v>24502</v>
       </c>
       <c r="G22" s="34" t="s">
@@ -10533,7 +10536,7 @@
       <c r="E23" s="36" t="s">
         <v>1586</v>
       </c>
-      <c r="F23" s="73">
+      <c r="F23" s="72">
         <v>18301</v>
       </c>
       <c r="G23" s="34" t="s">
@@ -10565,7 +10568,7 @@
       <c r="E24" s="36" t="s">
         <v>1519</v>
       </c>
-      <c r="F24" s="73">
+      <c r="F24" s="72">
         <v>41051</v>
       </c>
       <c r="G24" s="34" t="s">
@@ -10597,7 +10600,7 @@
       <c r="E25" s="36" t="s">
         <v>1578</v>
       </c>
-      <c r="F25" s="73">
+      <c r="F25" s="72">
         <v>29803</v>
       </c>
       <c r="G25" s="34" t="s">
@@ -10629,7 +10632,7 @@
       <c r="E26" s="36" t="s">
         <v>1530</v>
       </c>
-      <c r="F26" s="73">
+      <c r="F26" s="72">
         <v>22180</v>
       </c>
       <c r="G26" s="34" t="s">
@@ -10661,7 +10664,7 @@
       <c r="E27" s="48" t="s">
         <v>1519</v>
       </c>
-      <c r="F27" s="74">
+      <c r="F27" s="73">
         <v>20711</v>
       </c>
       <c r="G27" s="30" t="s">
@@ -10693,7 +10696,7 @@
       <c r="E28" s="48" t="s">
         <v>1594</v>
       </c>
-      <c r="F28" s="74">
+      <c r="F28" s="73">
         <v>27870</v>
       </c>
       <c r="G28" s="30" t="s">
@@ -10725,7 +10728,7 @@
       <c r="E29" s="48" t="s">
         <v>1578</v>
       </c>
-      <c r="F29" s="74">
+      <c r="F29" s="73">
         <v>29576</v>
       </c>
       <c r="G29" s="30" t="s">
@@ -10757,7 +10760,7 @@
       <c r="E30" s="48" t="s">
         <v>1598</v>
       </c>
-      <c r="F30" s="74">
+      <c r="F30" s="73">
         <v>60181</v>
       </c>
       <c r="G30" s="30" t="s">
@@ -10789,7 +10792,7 @@
       <c r="E31" s="48" t="s">
         <v>1561</v>
       </c>
-      <c r="F31" s="74">
+      <c r="F31" s="73">
         <v>90403</v>
       </c>
       <c r="G31" s="30" t="s">
@@ -10821,7 +10824,7 @@
       <c r="E32" s="36" t="s">
         <v>1519</v>
       </c>
-      <c r="F32" s="73">
+      <c r="F32" s="72">
         <v>21113</v>
       </c>
       <c r="G32" s="37" t="s">
@@ -10853,7 +10856,7 @@
       <c r="E33" s="36" t="s">
         <v>1564</v>
       </c>
-      <c r="F33" s="73">
+      <c r="F33" s="72">
         <v>32708</v>
       </c>
       <c r="G33" s="37" t="s">
@@ -10885,7 +10888,7 @@
       <c r="E34" s="36" t="s">
         <v>1561</v>
       </c>
-      <c r="F34" s="73">
+      <c r="F34" s="72">
         <v>44024</v>
       </c>
       <c r="G34" s="37" t="s">
@@ -10917,7 +10920,7 @@
       <c r="E35" s="36" t="s">
         <v>1603</v>
       </c>
-      <c r="F35" s="75">
+      <c r="F35" s="74">
         <v>1085</v>
       </c>
       <c r="G35" s="37" t="s">
@@ -10949,7 +10952,7 @@
       <c r="E36" s="36" t="s">
         <v>1594</v>
       </c>
-      <c r="F36" s="73">
+      <c r="F36" s="72">
         <v>27909</v>
       </c>
       <c r="G36" s="37" t="s">
@@ -10981,7 +10984,7 @@
       <c r="E37" s="48" t="s">
         <v>1519</v>
       </c>
-      <c r="F37" s="74">
+      <c r="F37" s="73">
         <v>63103</v>
       </c>
       <c r="G37" s="30" t="s">
@@ -11013,7 +11016,7 @@
       <c r="E38" s="48" t="s">
         <v>1607</v>
       </c>
-      <c r="F38" s="74">
+      <c r="F38" s="73">
         <v>8540</v>
       </c>
       <c r="G38" s="30" t="s">
@@ -11045,7 +11048,7 @@
       <c r="E39" s="48" t="s">
         <v>1530</v>
       </c>
-      <c r="F39" s="74">
+      <c r="F39" s="73">
         <v>84203</v>
       </c>
       <c r="G39" s="30" t="s">
@@ -11077,7 +11080,7 @@
       <c r="E40" s="48" t="s">
         <v>1561</v>
       </c>
-      <c r="F40" s="74">
+      <c r="F40" s="73">
         <v>44139</v>
       </c>
       <c r="G40" s="30" t="s">
@@ -11109,7 +11112,7 @@
       <c r="E41" s="48" t="s">
         <v>1555</v>
       </c>
-      <c r="F41" s="74">
+      <c r="F41" s="73">
         <v>98037</v>
       </c>
       <c r="G41" s="30" t="s">
@@ -11141,7 +11144,7 @@
       <c r="E42" s="36" t="s">
         <v>1519</v>
       </c>
-      <c r="F42" s="73">
+      <c r="F42" s="72">
         <v>21716</v>
       </c>
       <c r="G42" s="37" t="s">
@@ -11173,7 +11176,7 @@
       <c r="E43" s="36" t="s">
         <v>1586</v>
       </c>
-      <c r="F43" s="73">
+      <c r="F43" s="72">
         <v>15146</v>
       </c>
       <c r="G43" s="37" t="s">
@@ -11205,7 +11208,7 @@
       <c r="E44" s="36" t="s">
         <v>1586</v>
       </c>
-      <c r="F44" s="73">
+      <c r="F44" s="72">
         <v>15401</v>
       </c>
       <c r="G44" s="37" t="s">
@@ -11237,7 +11240,7 @@
       <c r="E45" s="36" t="s">
         <v>1607</v>
       </c>
-      <c r="F45" s="73">
+      <c r="F45" s="72">
         <v>7080</v>
       </c>
       <c r="G45" s="37" t="s">
@@ -11269,7 +11272,7 @@
       <c r="E46" s="36" t="s">
         <v>1558</v>
       </c>
-      <c r="F46" s="73">
+      <c r="F46" s="72">
         <v>11364</v>
       </c>
       <c r="G46" s="37" t="s">
@@ -11301,7 +11304,7 @@
       <c r="E47" s="48" t="s">
         <v>1519</v>
       </c>
-      <c r="F47" s="74">
+      <c r="F47" s="73">
         <v>21685</v>
       </c>
       <c r="G47" s="30" t="s">
@@ -11333,7 +11336,7 @@
       <c r="E48" s="48" t="s">
         <v>1564</v>
       </c>
-      <c r="F48" s="74">
+      <c r="F48" s="73">
         <v>32043</v>
       </c>
       <c r="G48" s="30" t="s">
@@ -11365,7 +11368,7 @@
       <c r="E49" s="48" t="s">
         <v>1574</v>
       </c>
-      <c r="F49" s="74">
+      <c r="F49" s="73">
         <v>30127</v>
       </c>
       <c r="G49" s="30" t="s">
@@ -11397,7 +11400,7 @@
       <c r="E50" s="48" t="s">
         <v>1603</v>
       </c>
-      <c r="F50" s="74">
+      <c r="F50" s="73">
         <v>2135</v>
       </c>
       <c r="G50" s="30" t="s">
@@ -11429,7 +11432,7 @@
       <c r="E51" s="48" t="s">
         <v>1555</v>
       </c>
-      <c r="F51" s="74">
+      <c r="F51" s="73">
         <v>46614</v>
       </c>
       <c r="G51" s="30" t="s">
@@ -11461,7 +11464,7 @@
       <c r="E52" s="36" t="s">
         <v>1519</v>
       </c>
-      <c r="F52" s="73">
+      <c r="F52" s="72">
         <v>21709</v>
       </c>
       <c r="G52" s="34" t="s">
@@ -11493,7 +11496,7 @@
       <c r="E53" s="36" t="s">
         <v>1586</v>
       </c>
-      <c r="F53" s="73">
+      <c r="F53" s="72">
         <v>19038</v>
       </c>
       <c r="G53" s="34" t="s">
@@ -11525,7 +11528,7 @@
       <c r="E54" s="36" t="s">
         <v>1555</v>
       </c>
-      <c r="F54" s="73">
+      <c r="F54" s="72">
         <v>44663</v>
       </c>
       <c r="G54" s="37" t="s">
@@ -11557,7 +11560,7 @@
       <c r="E55" s="36" t="s">
         <v>1530</v>
       </c>
-      <c r="F55" s="73">
+      <c r="F55" s="72">
         <v>98512</v>
       </c>
       <c r="G55" s="34" t="s">
@@ -11589,7 +11592,7 @@
       <c r="E56" s="36" t="s">
         <v>1586</v>
       </c>
-      <c r="F56" s="73">
+      <c r="F56" s="72">
         <v>19038</v>
       </c>
       <c r="G56" s="34" t="s">
@@ -11621,7 +11624,7 @@
       <c r="E57" s="48" t="s">
         <v>1607</v>
       </c>
-      <c r="F57" s="74">
+      <c r="F57" s="73">
         <v>8052</v>
       </c>
       <c r="G57" s="30" t="s">
@@ -11653,7 +11656,7 @@
       <c r="E58" s="48" t="s">
         <v>1564</v>
       </c>
-      <c r="F58" s="74">
+      <c r="F58" s="73">
         <v>33823</v>
       </c>
       <c r="G58" s="30" t="s">
@@ -11685,7 +11688,7 @@
       <c r="E59" s="48" t="s">
         <v>1586</v>
       </c>
-      <c r="F59" s="74">
+      <c r="F59" s="73">
         <v>17201</v>
       </c>
       <c r="G59" s="30" t="s">
@@ -11717,7 +11720,7 @@
       <c r="E60" s="48" t="s">
         <v>1555</v>
       </c>
-      <c r="F60" s="74">
+      <c r="F60" s="73">
         <v>46350</v>
       </c>
       <c r="G60" s="30" t="s">
@@ -11749,7 +11752,7 @@
       <c r="E61" s="48" t="s">
         <v>1607</v>
       </c>
-      <c r="F61" s="74">
+      <c r="F61" s="73">
         <v>8401</v>
       </c>
       <c r="G61" s="30" t="s">
@@ -11781,7 +11784,7 @@
       <c r="E62" s="36" t="s">
         <v>1519</v>
       </c>
-      <c r="F62" s="73">
+      <c r="F62" s="72">
         <v>20824</v>
       </c>
       <c r="G62" s="37" t="s">
@@ -11813,7 +11816,7 @@
       <c r="E63" s="36" t="s">
         <v>1519</v>
       </c>
-      <c r="F63" s="73">
+      <c r="F63" s="72">
         <v>20746</v>
       </c>
       <c r="G63" s="34" t="s">
@@ -11845,7 +11848,7 @@
       <c r="E64" s="36" t="s">
         <v>1558</v>
       </c>
-      <c r="F64" s="73">
+      <c r="F64" s="72">
         <v>11368</v>
       </c>
       <c r="G64" s="34" t="s">
@@ -11877,7 +11880,7 @@
       <c r="E65" s="36" t="s">
         <v>1561</v>
       </c>
-      <c r="F65" s="73">
+      <c r="F65" s="72">
         <v>44312</v>
       </c>
       <c r="G65" s="34" t="s">
@@ -11909,7 +11912,7 @@
       <c r="E66" s="36" t="s">
         <v>1603</v>
       </c>
-      <c r="F66" s="73">
+      <c r="F66" s="72">
         <v>1085</v>
       </c>
       <c r="G66" s="34" t="s">
@@ -11941,7 +11944,7 @@
       <c r="E67" s="48" t="s">
         <v>1519</v>
       </c>
-      <c r="F67" s="74">
+      <c r="F67" s="73">
         <v>20612</v>
       </c>
       <c r="G67" s="28" t="s">
@@ -11973,7 +11976,7 @@
       <c r="E68" s="48" t="s">
         <v>1555</v>
       </c>
-      <c r="F68" s="74">
+      <c r="F68" s="73">
         <v>54220</v>
       </c>
       <c r="G68" s="28" t="s">
@@ -12005,7 +12008,7 @@
       <c r="E69" s="48" t="s">
         <v>1530</v>
       </c>
-      <c r="F69" s="74">
+      <c r="F69" s="73">
         <v>23832</v>
       </c>
       <c r="G69" s="28" t="s">
@@ -12037,7 +12040,7 @@
       <c r="E70" s="48" t="s">
         <v>1558</v>
       </c>
-      <c r="F70" s="74">
+      <c r="F70" s="73">
         <v>11377</v>
       </c>
       <c r="G70" s="30" t="s">
@@ -12069,7 +12072,7 @@
       <c r="E71" s="48" t="s">
         <v>1586</v>
       </c>
-      <c r="F71" s="74">
+      <c r="F71" s="73">
         <v>48071</v>
       </c>
       <c r="G71" s="30" t="s">
@@ -12101,7 +12104,7 @@
       <c r="E72" s="36" t="s">
         <v>1519</v>
       </c>
-      <c r="F72" s="73">
+      <c r="F72" s="72">
         <v>21052</v>
       </c>
       <c r="G72" s="34" t="s">
@@ -12133,7 +12136,7 @@
       <c r="E73" s="36" t="s">
         <v>1586</v>
       </c>
-      <c r="F73" s="73">
+      <c r="F73" s="72">
         <v>54650</v>
       </c>
       <c r="G73" s="34" t="s">
@@ -12165,7 +12168,7 @@
       <c r="E74" s="36" t="s">
         <v>1607</v>
       </c>
-      <c r="F74" s="73">
+      <c r="F74" s="72">
         <v>8012</v>
       </c>
       <c r="G74" s="34" t="s">
@@ -12197,7 +12200,7 @@
       <c r="E75" s="36" t="s">
         <v>1519</v>
       </c>
-      <c r="F75" s="73">
+      <c r="F75" s="72">
         <v>78213</v>
       </c>
       <c r="G75" s="37" t="s">
@@ -12229,7 +12232,7 @@
       <c r="E76" s="36" t="s">
         <v>1603</v>
       </c>
-      <c r="F76" s="73">
+      <c r="F76" s="72">
         <v>1821</v>
       </c>
       <c r="G76" s="34" t="s">
@@ -12261,7 +12264,7 @@
       <c r="E77" s="48" t="s">
         <v>1519</v>
       </c>
-      <c r="F77" s="74">
+      <c r="F77" s="73">
         <v>21014</v>
       </c>
       <c r="G77" s="30" t="s">
@@ -12293,7 +12296,7 @@
       <c r="E78" s="48" t="s">
         <v>1594</v>
       </c>
-      <c r="F78" s="74">
+      <c r="F78" s="73">
         <v>25787</v>
       </c>
       <c r="G78" s="28" t="s">
@@ -12325,7 +12328,7 @@
       <c r="E79" s="48" t="s">
         <v>1519</v>
       </c>
-      <c r="F79" s="74">
+      <c r="F79" s="73">
         <v>75126</v>
       </c>
       <c r="G79" s="28" t="s">
@@ -12357,7 +12360,7 @@
       <c r="E80" s="48" t="s">
         <v>1574</v>
       </c>
-      <c r="F80" s="74">
+      <c r="F80" s="73">
         <v>30721</v>
       </c>
       <c r="G80" s="28" t="s">
@@ -12389,7 +12392,7 @@
       <c r="E81" s="48" t="s">
         <v>1607</v>
       </c>
-      <c r="F81" s="74">
+      <c r="F81" s="73">
         <v>8037</v>
       </c>
       <c r="G81" s="30" t="s">
@@ -12421,7 +12424,7 @@
       <c r="E82" s="36" t="s">
         <v>1519</v>
       </c>
-      <c r="F82" s="73">
+      <c r="F82" s="72">
         <v>20747</v>
       </c>
       <c r="G82" s="37" t="s">
@@ -12453,7 +12456,7 @@
       <c r="E83" s="36" t="s">
         <v>1603</v>
       </c>
-      <c r="F83" s="73">
+      <c r="F83" s="72">
         <v>2127</v>
       </c>
       <c r="G83" s="34" t="s">
@@ -12485,7 +12488,7 @@
       <c r="E84" s="36" t="s">
         <v>1530</v>
       </c>
-      <c r="F84" s="73">
+      <c r="F84" s="72">
         <v>53072</v>
       </c>
       <c r="G84" s="34" t="s">
@@ -12517,7 +12520,7 @@
       <c r="E85" s="36" t="s">
         <v>1567</v>
       </c>
-      <c r="F85" s="73">
+      <c r="F85" s="72">
         <v>6824</v>
       </c>
       <c r="G85" s="34" t="s">
@@ -12549,7 +12552,7 @@
       <c r="E86" s="36" t="s">
         <v>1607</v>
       </c>
-      <c r="F86" s="73">
+      <c r="F86" s="72">
         <v>8088</v>
       </c>
       <c r="G86" s="37" t="s">
@@ -12581,7 +12584,7 @@
       <c r="E87" s="48" t="s">
         <v>1519</v>
       </c>
-      <c r="F87" s="74">
+      <c r="F87" s="73">
         <v>20680</v>
       </c>
       <c r="G87" s="28" t="s">
@@ -12613,7 +12616,7 @@
       <c r="E88" s="48" t="s">
         <v>1558</v>
       </c>
-      <c r="F88" s="74">
+      <c r="F88" s="73">
         <v>11803</v>
       </c>
       <c r="G88" s="28" t="s">
@@ -12645,7 +12648,7 @@
       <c r="E89" s="48" t="s">
         <v>1555</v>
       </c>
-      <c r="F89" s="74">
+      <c r="F89" s="73">
         <v>47150</v>
       </c>
       <c r="G89" s="28" t="s">
@@ -12677,7 +12680,7 @@
       <c r="E90" s="48" t="s">
         <v>1586</v>
       </c>
-      <c r="F90" s="74">
+      <c r="F90" s="73">
         <v>17022</v>
       </c>
       <c r="G90" s="28" t="s">
@@ -12709,7 +12712,7 @@
       <c r="E91" s="48" t="s">
         <v>1555</v>
       </c>
-      <c r="F91" s="74">
+      <c r="F91" s="73">
         <v>60172</v>
       </c>
       <c r="G91" s="28" t="s">
@@ -12741,7 +12744,7 @@
       <c r="E92" s="36" t="s">
         <v>1519</v>
       </c>
-      <c r="F92" s="73">
+      <c r="F92" s="72">
         <v>21219</v>
       </c>
       <c r="G92" s="37" t="s">
@@ -12773,7 +12776,7 @@
       <c r="E93" s="36" t="s">
         <v>1567</v>
       </c>
-      <c r="F93" s="73">
+      <c r="F93" s="72">
         <v>6902</v>
       </c>
       <c r="G93" s="34" t="s">
@@ -12805,7 +12808,7 @@
       <c r="E94" s="36" t="s">
         <v>1519</v>
       </c>
-      <c r="F94" s="73">
+      <c r="F94" s="72">
         <v>90274</v>
       </c>
       <c r="G94" s="37" t="s">
@@ -12837,7 +12840,7 @@
       <c r="E95" s="36" t="s">
         <v>1586</v>
       </c>
-      <c r="F95" s="73">
+      <c r="F95" s="72">
         <v>54952</v>
       </c>
       <c r="G95" s="37" t="s">
@@ -12869,7 +12872,7 @@
       <c r="E96" s="36" t="s">
         <v>1578</v>
       </c>
-      <c r="F96" s="73">
+      <c r="F96" s="72">
         <v>29710</v>
       </c>
       <c r="G96" s="40" t="s">
@@ -15493,7 +15496,7 @@
   <dimension ref="A1:O77"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15585,11 +15588,11 @@
       <c r="G2" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="H2" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I2" s="11">
-        <v>43560</v>
+      <c r="H2" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I2" s="75">
+        <v>43589</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>250</v>
@@ -15629,11 +15632,11 @@
       <c r="G3" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="H3" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I3" s="11">
-        <v>43560</v>
+      <c r="H3" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I3" s="75">
+        <v>43589</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>249</v>
@@ -15673,11 +15676,11 @@
       <c r="G4" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="H4" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I4" s="11">
-        <v>43560</v>
+      <c r="H4" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I4" s="75">
+        <v>43589</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>249</v>
@@ -15717,11 +15720,11 @@
       <c r="G5" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="H5" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I5" s="11">
-        <v>43560</v>
+      <c r="H5" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I5" s="75">
+        <v>43589</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>248</v>
@@ -15761,11 +15764,11 @@
       <c r="G6" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="H6" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I6" s="11">
-        <v>43560</v>
+      <c r="H6" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I6" s="75">
+        <v>43589</v>
       </c>
       <c r="J6" s="11" t="s">
         <v>248</v>
@@ -15805,11 +15808,11 @@
       <c r="G7" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="H7" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I7" s="11">
-        <v>43560</v>
+      <c r="H7" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I7" s="75">
+        <v>43589</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>248</v>
@@ -15849,11 +15852,11 @@
       <c r="G8" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="H8" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I8" s="11">
-        <v>43560</v>
+      <c r="H8" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I8" s="75">
+        <v>43589</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>248</v>
@@ -15893,11 +15896,11 @@
       <c r="G9" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="H9" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I9" s="11">
-        <v>43560</v>
+      <c r="H9" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I9" s="75">
+        <v>43589</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>250</v>
@@ -15937,11 +15940,11 @@
       <c r="G10" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="H10" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I10" s="11">
-        <v>43560</v>
+      <c r="H10" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I10" s="75">
+        <v>43589</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>249</v>
@@ -15981,11 +15984,11 @@
       <c r="G11" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="H11" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I11" s="11">
-        <v>43560</v>
+      <c r="H11" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I11" s="75">
+        <v>43589</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>249</v>
@@ -16025,11 +16028,11 @@
       <c r="G12" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="H12" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I12" s="11">
-        <v>43560</v>
+      <c r="H12" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I12" s="75">
+        <v>43589</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>250</v>
@@ -16069,11 +16072,11 @@
       <c r="G13" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="H13" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I13" s="11">
-        <v>43560</v>
+      <c r="H13" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I13" s="75">
+        <v>43589</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>250</v>
@@ -16113,11 +16116,11 @@
       <c r="G14" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="H14" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I14" s="11">
-        <v>43560</v>
+      <c r="H14" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I14" s="75">
+        <v>43589</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>250</v>
@@ -16157,11 +16160,11 @@
       <c r="G15" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="H15" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I15" s="11">
-        <v>43560</v>
+      <c r="H15" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I15" s="75">
+        <v>43589</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>249</v>
@@ -16201,11 +16204,11 @@
       <c r="G16" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="H16" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I16" s="11">
-        <v>43560</v>
+      <c r="H16" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I16" s="75">
+        <v>43589</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>249</v>
@@ -16245,11 +16248,11 @@
       <c r="G17" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="H17" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I17" s="11">
-        <v>43560</v>
+      <c r="H17" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I17" s="75">
+        <v>43589</v>
       </c>
       <c r="J17" s="11" t="s">
         <v>248</v>
@@ -16289,11 +16292,11 @@
       <c r="G18" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="H18" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I18" s="11">
-        <v>43560</v>
+      <c r="H18" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I18" s="75">
+        <v>43589</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>250</v>
@@ -16333,11 +16336,11 @@
       <c r="G19" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="H19" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I19" s="11">
-        <v>43560</v>
+      <c r="H19" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I19" s="75">
+        <v>43589</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>249</v>
@@ -16377,11 +16380,11 @@
       <c r="G20" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="H20" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I20" s="11">
-        <v>43560</v>
+      <c r="H20" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I20" s="75">
+        <v>43589</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>249</v>
@@ -16421,11 +16424,11 @@
       <c r="G21" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="H21" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I21" s="11">
-        <v>43560</v>
+      <c r="H21" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I21" s="75">
+        <v>43589</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>250</v>
@@ -16465,11 +16468,11 @@
       <c r="G22" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="H22" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I22" s="11">
-        <v>43560</v>
+      <c r="H22" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I22" s="75">
+        <v>43589</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>248</v>
@@ -16509,11 +16512,11 @@
       <c r="G23" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="H23" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I23" s="11">
-        <v>43560</v>
+      <c r="H23" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I23" s="75">
+        <v>43589</v>
       </c>
       <c r="J23" s="11" t="s">
         <v>248</v>
@@ -16553,11 +16556,11 @@
       <c r="G24" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="H24" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I24" s="11">
-        <v>43560</v>
+      <c r="H24" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I24" s="75">
+        <v>43589</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>250</v>
@@ -16597,11 +16600,11 @@
       <c r="G25" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="H25" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I25" s="11">
-        <v>43560</v>
+      <c r="H25" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I25" s="75">
+        <v>43589</v>
       </c>
       <c r="J25" s="11" t="s">
         <v>249</v>
@@ -16641,11 +16644,11 @@
       <c r="G26" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="H26" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I26" s="11">
-        <v>43560</v>
+      <c r="H26" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I26" s="75">
+        <v>43589</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>249</v>
@@ -16685,11 +16688,11 @@
       <c r="G27" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="H27" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I27" s="11">
-        <v>43560</v>
+      <c r="H27" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I27" s="75">
+        <v>43589</v>
       </c>
       <c r="J27" s="11" t="s">
         <v>248</v>
@@ -16729,11 +16732,11 @@
       <c r="G28" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="H28" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I28" s="11">
-        <v>43560</v>
+      <c r="H28" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I28" s="75">
+        <v>43589</v>
       </c>
       <c r="J28" s="11" t="s">
         <v>248</v>
@@ -16773,11 +16776,11 @@
       <c r="G29" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="H29" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I29" s="11">
-        <v>43560</v>
+      <c r="H29" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I29" s="75">
+        <v>43589</v>
       </c>
       <c r="J29" s="11" t="s">
         <v>248</v>
@@ -16817,11 +16820,11 @@
       <c r="G30" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="H30" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I30" s="11">
-        <v>43560</v>
+      <c r="H30" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I30" s="75">
+        <v>43589</v>
       </c>
       <c r="J30" s="11" t="s">
         <v>250</v>
@@ -16861,11 +16864,11 @@
       <c r="G31" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="H31" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I31" s="11">
-        <v>43560</v>
+      <c r="H31" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I31" s="75">
+        <v>43589</v>
       </c>
       <c r="J31" s="11" t="s">
         <v>249</v>
@@ -16905,11 +16908,11 @@
       <c r="G32" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="H32" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I32" s="11">
-        <v>43560</v>
+      <c r="H32" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I32" s="75">
+        <v>43589</v>
       </c>
       <c r="J32" s="11" t="s">
         <v>249</v>
@@ -16949,11 +16952,11 @@
       <c r="G33" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="H33" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I33" s="11">
-        <v>43560</v>
+      <c r="H33" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I33" s="75">
+        <v>43589</v>
       </c>
       <c r="J33" s="11" t="s">
         <v>248</v>
@@ -16993,11 +16996,11 @@
       <c r="G34" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="H34" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I34" s="11">
-        <v>43560</v>
+      <c r="H34" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I34" s="75">
+        <v>43589</v>
       </c>
       <c r="J34" s="11" t="s">
         <v>248</v>
@@ -17037,11 +17040,11 @@
       <c r="G35" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="H35" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I35" s="11">
-        <v>43560</v>
+      <c r="H35" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I35" s="75">
+        <v>43589</v>
       </c>
       <c r="J35" s="11" t="s">
         <v>248</v>
@@ -17081,11 +17084,11 @@
       <c r="G36" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="H36" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I36" s="11">
-        <v>43560</v>
+      <c r="H36" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I36" s="75">
+        <v>43589</v>
       </c>
       <c r="J36" s="11" t="s">
         <v>250</v>
@@ -17125,11 +17128,11 @@
       <c r="G37" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="H37" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I37" s="11">
-        <v>43560</v>
+      <c r="H37" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I37" s="75">
+        <v>43589</v>
       </c>
       <c r="J37" s="11" t="s">
         <v>249</v>
@@ -17169,11 +17172,11 @@
       <c r="G38" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="H38" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I38" s="11">
-        <v>43560</v>
+      <c r="H38" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I38" s="75">
+        <v>43589</v>
       </c>
       <c r="J38" s="11" t="s">
         <v>249</v>
@@ -17213,11 +17216,11 @@
       <c r="G39" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="H39" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I39" s="11">
-        <v>43560</v>
+      <c r="H39" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I39" s="75">
+        <v>43589</v>
       </c>
       <c r="J39" s="11" t="s">
         <v>248</v>
@@ -17257,11 +17260,11 @@
       <c r="G40" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="H40" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I40" s="11">
-        <v>43560</v>
+      <c r="H40" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I40" s="75">
+        <v>43589</v>
       </c>
       <c r="J40" s="11" t="s">
         <v>248</v>
@@ -17301,11 +17304,11 @@
       <c r="G41" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="H41" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I41" s="11">
-        <v>43560</v>
+      <c r="H41" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I41" s="75">
+        <v>43589</v>
       </c>
       <c r="J41" s="11" t="s">
         <v>248</v>
@@ -17345,11 +17348,11 @@
       <c r="G42" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="H42" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I42" s="11">
-        <v>43560</v>
+      <c r="H42" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I42" s="75">
+        <v>43589</v>
       </c>
       <c r="J42" s="11" t="s">
         <v>250</v>
@@ -17389,11 +17392,11 @@
       <c r="G43" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="H43" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I43" s="11">
-        <v>43560</v>
+      <c r="H43" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I43" s="75">
+        <v>43589</v>
       </c>
       <c r="J43" s="11" t="s">
         <v>249</v>
@@ -17433,11 +17436,11 @@
       <c r="G44" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="H44" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I44" s="11">
-        <v>43560</v>
+      <c r="H44" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I44" s="75">
+        <v>43589</v>
       </c>
       <c r="J44" s="11" t="s">
         <v>249</v>
@@ -17477,11 +17480,11 @@
       <c r="G45" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="H45" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I45" s="11">
-        <v>43560</v>
+      <c r="H45" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I45" s="75">
+        <v>43589</v>
       </c>
       <c r="J45" s="11" t="s">
         <v>248</v>
@@ -17521,11 +17524,11 @@
       <c r="G46" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="H46" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I46" s="11">
-        <v>43560</v>
+      <c r="H46" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I46" s="75">
+        <v>43589</v>
       </c>
       <c r="J46" s="11" t="s">
         <v>248</v>
@@ -17565,11 +17568,11 @@
       <c r="G47" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="H47" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I47" s="11">
-        <v>43560</v>
+      <c r="H47" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I47" s="75">
+        <v>43589</v>
       </c>
       <c r="J47" s="11" t="s">
         <v>248</v>
@@ -17609,11 +17612,11 @@
       <c r="G48" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="H48" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I48" s="11">
-        <v>43560</v>
+      <c r="H48" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I48" s="75">
+        <v>43589</v>
       </c>
       <c r="J48" s="11" t="s">
         <v>250</v>
@@ -17653,11 +17656,11 @@
       <c r="G49" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="H49" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I49" s="11">
-        <v>43560</v>
+      <c r="H49" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I49" s="75">
+        <v>43589</v>
       </c>
       <c r="J49" s="11" t="s">
         <v>249</v>
@@ -17697,11 +17700,11 @@
       <c r="G50" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="H50" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I50" s="11">
-        <v>43560</v>
+      <c r="H50" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I50" s="75">
+        <v>43589</v>
       </c>
       <c r="J50" s="11" t="s">
         <v>249</v>
@@ -17741,11 +17744,11 @@
       <c r="G51" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="H51" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I51" s="11">
-        <v>43560</v>
+      <c r="H51" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I51" s="75">
+        <v>43589</v>
       </c>
       <c r="J51" s="11" t="s">
         <v>248</v>
@@ -17785,11 +17788,11 @@
       <c r="G52" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="H52" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I52" s="11">
-        <v>43560</v>
+      <c r="H52" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I52" s="75">
+        <v>43589</v>
       </c>
       <c r="J52" s="11" t="s">
         <v>248</v>
@@ -17829,11 +17832,11 @@
       <c r="G53" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="H53" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I53" s="11">
-        <v>43560</v>
+      <c r="H53" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I53" s="75">
+        <v>43589</v>
       </c>
       <c r="J53" s="11" t="s">
         <v>248</v>
@@ -17873,11 +17876,11 @@
       <c r="G54" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="H54" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I54" s="11">
-        <v>43560</v>
+      <c r="H54" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I54" s="75">
+        <v>43589</v>
       </c>
       <c r="J54" s="11" t="s">
         <v>250</v>
@@ -17917,11 +17920,11 @@
       <c r="G55" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="H55" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I55" s="11">
-        <v>43560</v>
+      <c r="H55" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I55" s="75">
+        <v>43589</v>
       </c>
       <c r="J55" s="11" t="s">
         <v>249</v>
@@ -17961,11 +17964,11 @@
       <c r="G56" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="H56" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I56" s="11">
-        <v>43560</v>
+      <c r="H56" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I56" s="75">
+        <v>43589</v>
       </c>
       <c r="J56" s="11" t="s">
         <v>249</v>
@@ -18005,11 +18008,11 @@
       <c r="G57" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="H57" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I57" s="11">
-        <v>43560</v>
+      <c r="H57" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I57" s="75">
+        <v>43589</v>
       </c>
       <c r="J57" s="11" t="s">
         <v>248</v>
@@ -18049,11 +18052,11 @@
       <c r="G58" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="H58" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I58" s="11">
-        <v>43560</v>
+      <c r="H58" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I58" s="75">
+        <v>43589</v>
       </c>
       <c r="J58" s="11" t="s">
         <v>248</v>
@@ -18093,11 +18096,11 @@
       <c r="G59" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="H59" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I59" s="11">
-        <v>43560</v>
+      <c r="H59" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I59" s="75">
+        <v>43589</v>
       </c>
       <c r="J59" s="11" t="s">
         <v>248</v>
@@ -18137,11 +18140,11 @@
       <c r="G60" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="H60" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I60" s="11">
-        <v>43560</v>
+      <c r="H60" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I60" s="75">
+        <v>43589</v>
       </c>
       <c r="J60" s="11" t="s">
         <v>250</v>
@@ -18181,11 +18184,11 @@
       <c r="G61" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="H61" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I61" s="11">
-        <v>43560</v>
+      <c r="H61" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I61" s="75">
+        <v>43589</v>
       </c>
       <c r="J61" s="11" t="s">
         <v>249</v>
@@ -18225,11 +18228,11 @@
       <c r="G62" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="H62" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I62" s="11">
-        <v>43560</v>
+      <c r="H62" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I62" s="75">
+        <v>43589</v>
       </c>
       <c r="J62" s="11" t="s">
         <v>249</v>
@@ -18269,11 +18272,11 @@
       <c r="G63" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="H63" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I63" s="11">
-        <v>43560</v>
+      <c r="H63" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I63" s="75">
+        <v>43589</v>
       </c>
       <c r="J63" s="11" t="s">
         <v>248</v>
@@ -18313,11 +18316,11 @@
       <c r="G64" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="H64" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I64" s="11">
-        <v>43560</v>
+      <c r="H64" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I64" s="75">
+        <v>43589</v>
       </c>
       <c r="J64" s="11" t="s">
         <v>248</v>
@@ -18357,11 +18360,11 @@
       <c r="G65" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="H65" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I65" s="11">
-        <v>43560</v>
+      <c r="H65" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I65" s="75">
+        <v>43589</v>
       </c>
       <c r="J65" s="11" t="s">
         <v>248</v>
@@ -18401,11 +18404,11 @@
       <c r="G66" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="H66" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I66" s="11">
-        <v>43560</v>
+      <c r="H66" s="75">
+        <v>43224</v>
+      </c>
+      <c r="I66" s="75">
+        <v>43589</v>
       </c>
       <c r="J66" s="11" t="s">
         <v>248</v>
@@ -18445,11 +18448,11 @@
       <c r="G67" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="H67" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I67" s="11">
-        <v>43560</v>
+      <c r="H67" s="75">
+        <v>43255</v>
+      </c>
+      <c r="I67" s="75">
+        <v>43620</v>
       </c>
       <c r="J67" s="11" t="s">
         <v>250</v>
@@ -18489,11 +18492,11 @@
       <c r="G68" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="H68" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I68" s="11">
-        <v>43560</v>
+      <c r="H68" s="75">
+        <v>43285</v>
+      </c>
+      <c r="I68" s="75">
+        <v>43650</v>
       </c>
       <c r="J68" s="11" t="s">
         <v>249</v>
@@ -18533,11 +18536,11 @@
       <c r="G69" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="H69" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I69" s="11">
-        <v>43560</v>
+      <c r="H69" s="75">
+        <v>43316</v>
+      </c>
+      <c r="I69" s="75">
+        <v>43681</v>
       </c>
       <c r="J69" s="11" t="s">
         <v>249</v>
@@ -18577,11 +18580,11 @@
       <c r="G70" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="H70" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I70" s="11">
-        <v>43560</v>
+      <c r="H70" s="75">
+        <v>43347</v>
+      </c>
+      <c r="I70" s="75">
+        <v>43712</v>
       </c>
       <c r="J70" s="11" t="s">
         <v>250</v>
@@ -18621,11 +18624,11 @@
       <c r="G71" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="H71" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I71" s="11">
-        <v>43560</v>
+      <c r="H71" s="75">
+        <v>43377</v>
+      </c>
+      <c r="I71" s="75">
+        <v>43742</v>
       </c>
       <c r="J71" s="11" t="s">
         <v>248</v>
@@ -18665,11 +18668,11 @@
       <c r="G72" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="H72" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I72" s="11">
-        <v>43560</v>
+      <c r="H72" s="75">
+        <v>43408</v>
+      </c>
+      <c r="I72" s="75">
+        <v>43773</v>
       </c>
       <c r="J72" s="11" t="s">
         <v>248</v>
@@ -18709,11 +18712,11 @@
       <c r="G73" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="H73" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I73" s="11">
-        <v>43560</v>
+      <c r="H73" s="75">
+        <v>43438</v>
+      </c>
+      <c r="I73" s="75">
+        <v>43803</v>
       </c>
       <c r="J73" s="11" t="s">
         <v>250</v>
@@ -18753,11 +18756,11 @@
       <c r="G74" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="H74" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I74" s="11">
-        <v>43560</v>
+      <c r="H74" s="75">
+        <v>43439</v>
+      </c>
+      <c r="I74" s="75">
+        <v>43804</v>
       </c>
       <c r="J74" s="11" t="s">
         <v>249</v>
@@ -18797,11 +18800,11 @@
       <c r="G75" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="H75" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I75" s="11">
-        <v>43560</v>
+      <c r="H75" s="75">
+        <v>43440</v>
+      </c>
+      <c r="I75" s="75">
+        <v>43805</v>
       </c>
       <c r="J75" s="11" t="s">
         <v>249</v>
@@ -18841,11 +18844,11 @@
       <c r="G76" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="H76" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I76" s="11">
-        <v>43560</v>
+      <c r="H76" s="75">
+        <v>43441</v>
+      </c>
+      <c r="I76" s="75">
+        <v>43806</v>
       </c>
       <c r="J76" s="11" t="s">
         <v>250</v>
@@ -18885,11 +18888,11 @@
       <c r="G77" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="H77" s="11">
-        <v>43195</v>
-      </c>
-      <c r="I77" s="11">
-        <v>43560</v>
+      <c r="H77" s="75">
+        <v>43442</v>
+      </c>
+      <c r="I77" s="75">
+        <v>43807</v>
       </c>
       <c r="J77" s="11" t="s">
         <v>248</v>
@@ -18915,7 +18918,6 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:O99"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -18989,7 +18991,7 @@
         <v>1770</v>
       </c>
     </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="63" t="s">
         <v>93</v>
       </c>
@@ -19083,7 +19085,7 @@
         <v>1772</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
         <v>95</v>
       </c>
@@ -19130,7 +19132,7 @@
         <v>1773</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="64" t="s">
         <v>96</v>
       </c>
@@ -19177,7 +19179,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
         <v>97</v>
       </c>
@@ -19224,7 +19226,7 @@
         <v>1775</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
         <v>98</v>
       </c>
@@ -19271,7 +19273,7 @@
         <v>1776</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="64" t="s">
         <v>99</v>
       </c>
@@ -19318,7 +19320,7 @@
         <v>1777</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="64" t="s">
         <v>440</v>
       </c>
@@ -19365,7 +19367,7 @@
         <v>1778</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="64" t="s">
         <v>449</v>
       </c>
@@ -19412,7 +19414,7 @@
         <v>1779</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="64" t="s">
         <v>100</v>
       </c>
@@ -19459,7 +19461,7 @@
         <v>1780</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="64" t="s">
         <v>101</v>
       </c>
@@ -19506,7 +19508,7 @@
         <v>1789</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="64" t="s">
         <v>472</v>
       </c>
@@ -19553,7 +19555,7 @@
         <v>1781</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="64" t="s">
         <v>102</v>
       </c>
@@ -19600,7 +19602,7 @@
         <v>1782</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="64" t="s">
         <v>103</v>
       </c>
@@ -19647,7 +19649,7 @@
         <v>1783</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="64" t="s">
         <v>104</v>
       </c>
@@ -19694,7 +19696,7 @@
         <v>1784</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="64" t="s">
         <v>105</v>
       </c>
@@ -19741,7 +19743,7 @@
         <v>1785</v>
       </c>
     </row>
-    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="64" t="s">
         <v>106</v>
       </c>
@@ -19788,7 +19790,7 @@
         <v>1786</v>
       </c>
     </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="64" t="s">
         <v>107</v>
       </c>
@@ -19835,7 +19837,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="64" t="s">
         <v>108</v>
       </c>
@@ -19882,7 +19884,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="63" t="s">
         <v>93</v>
       </c>
@@ -19976,7 +19978,7 @@
         <v>1827</v>
       </c>
     </row>
-    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="64" t="s">
         <v>95</v>
       </c>
@@ -20023,7 +20025,7 @@
         <v>1828</v>
       </c>
     </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="64" t="s">
         <v>96</v>
       </c>
@@ -20070,7 +20072,7 @@
         <v>1829</v>
       </c>
     </row>
-    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="64" t="s">
         <v>97</v>
       </c>
@@ -20117,7 +20119,7 @@
         <v>1830</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="64" t="s">
         <v>98</v>
       </c>
@@ -20164,7 +20166,7 @@
         <v>1831</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="64" t="s">
         <v>99</v>
       </c>
@@ -20211,7 +20213,7 @@
         <v>1832</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="64" t="s">
         <v>440</v>
       </c>
@@ -20258,7 +20260,7 @@
         <v>1833</v>
       </c>
     </row>
-    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="64" t="s">
         <v>449</v>
       </c>
@@ -20305,7 +20307,7 @@
         <v>1834</v>
       </c>
     </row>
-    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="64" t="s">
         <v>100</v>
       </c>
@@ -20352,7 +20354,7 @@
         <v>1835</v>
       </c>
     </row>
-    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="64" t="s">
         <v>101</v>
       </c>
@@ -20399,7 +20401,7 @@
         <v>1836</v>
       </c>
     </row>
-    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="64" t="s">
         <v>472</v>
       </c>
@@ -20446,7 +20448,7 @@
         <v>1837</v>
       </c>
     </row>
-    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="64" t="s">
         <v>102</v>
       </c>
@@ -20493,7 +20495,7 @@
         <v>1838</v>
       </c>
     </row>
-    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="64" t="s">
         <v>103</v>
       </c>
@@ -20540,7 +20542,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="64" t="s">
         <v>104</v>
       </c>
@@ -20587,7 +20589,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="64" t="s">
         <v>105</v>
       </c>
@@ -20634,7 +20636,7 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="64" t="s">
         <v>106</v>
       </c>
@@ -20681,7 +20683,7 @@
         <v>1842</v>
       </c>
     </row>
-    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="64" t="s">
         <v>107</v>
       </c>
@@ -20728,7 +20730,7 @@
         <v>1843</v>
       </c>
     </row>
-    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="64" t="s">
         <v>108</v>
       </c>
@@ -20775,7 +20777,7 @@
         <v>1844</v>
       </c>
     </row>
-    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="63" t="s">
         <v>93</v>
       </c>
@@ -20869,7 +20871,7 @@
         <v>1865</v>
       </c>
     </row>
-    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="64" t="s">
         <v>95</v>
       </c>
@@ -20916,7 +20918,7 @@
         <v>1866</v>
       </c>
     </row>
-    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="64" t="s">
         <v>96</v>
       </c>
@@ -20963,7 +20965,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="64" t="s">
         <v>97</v>
       </c>
@@ -21010,7 +21012,7 @@
         <v>1868</v>
       </c>
     </row>
-    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="64" t="s">
         <v>98</v>
       </c>
@@ -21057,7 +21059,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="64" t="s">
         <v>99</v>
       </c>
@@ -21104,7 +21106,7 @@
         <v>1870</v>
       </c>
     </row>
-    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="64" t="s">
         <v>440</v>
       </c>
@@ -21151,7 +21153,7 @@
         <v>1845</v>
       </c>
     </row>
-    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="64" t="s">
         <v>449</v>
       </c>
@@ -21198,7 +21200,7 @@
         <v>1871</v>
       </c>
     </row>
-    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="64" t="s">
         <v>100</v>
       </c>
@@ -21245,7 +21247,7 @@
         <v>1872</v>
       </c>
     </row>
-    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="64" t="s">
         <v>101</v>
       </c>
@@ -21292,7 +21294,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="64" t="s">
         <v>472</v>
       </c>
@@ -21339,7 +21341,7 @@
         <v>1874</v>
       </c>
     </row>
-    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="64" t="s">
         <v>102</v>
       </c>
@@ -21386,7 +21388,7 @@
         <v>1875</v>
       </c>
     </row>
-    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="64" t="s">
         <v>103</v>
       </c>
@@ -21433,7 +21435,7 @@
         <v>1876</v>
       </c>
     </row>
-    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="64" t="s">
         <v>104</v>
       </c>
@@ -21480,7 +21482,7 @@
         <v>1877</v>
       </c>
     </row>
-    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="64" t="s">
         <v>105</v>
       </c>
@@ -21527,7 +21529,7 @@
         <v>1878</v>
       </c>
     </row>
-    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="64" t="s">
         <v>106</v>
       </c>
@@ -21574,7 +21576,7 @@
         <v>1879</v>
       </c>
     </row>
-    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="64" t="s">
         <v>107</v>
       </c>
@@ -21621,7 +21623,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="64" t="s">
         <v>108</v>
       </c>
@@ -21668,7 +21670,7 @@
         <v>1881</v>
       </c>
     </row>
-    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="63" t="s">
         <v>93</v>
       </c>
@@ -21762,7 +21764,7 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="64" t="s">
         <v>95</v>
       </c>
@@ -21809,7 +21811,7 @@
         <v>1846</v>
       </c>
     </row>
-    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="64" t="s">
         <v>96</v>
       </c>
@@ -21856,7 +21858,7 @@
         <v>1884</v>
       </c>
     </row>
-    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="64" t="s">
         <v>97</v>
       </c>
@@ -21903,7 +21905,7 @@
         <v>1885</v>
       </c>
     </row>
-    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="64" t="s">
         <v>98</v>
       </c>
@@ -21950,7 +21952,7 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="64" t="s">
         <v>99</v>
       </c>
@@ -21997,7 +21999,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="64" t="s">
         <v>440</v>
       </c>
@@ -22044,7 +22046,7 @@
         <v>1888</v>
       </c>
     </row>
-    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="64" t="s">
         <v>449</v>
       </c>
@@ -22091,7 +22093,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="64" t="s">
         <v>100</v>
       </c>
@@ -22138,7 +22140,7 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="64" t="s">
         <v>101</v>
       </c>
@@ -22185,7 +22187,7 @@
         <v>1889</v>
       </c>
     </row>
-    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="64" t="s">
         <v>472</v>
       </c>
@@ -22232,7 +22234,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="64" t="s">
         <v>102</v>
       </c>
@@ -22279,7 +22281,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="64" t="s">
         <v>103</v>
       </c>
@@ -22326,7 +22328,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="64" t="s">
         <v>104</v>
       </c>
@@ -22373,7 +22375,7 @@
         <v>1893</v>
       </c>
     </row>
-    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="64" t="s">
         <v>105</v>
       </c>
@@ -22420,7 +22422,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="64" t="s">
         <v>106</v>
       </c>
@@ -22467,7 +22469,7 @@
         <v>1895</v>
       </c>
     </row>
-    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="64" t="s">
         <v>107</v>
       </c>
@@ -22514,7 +22516,7 @@
         <v>1896</v>
       </c>
     </row>
-    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="64" t="s">
         <v>108</v>
       </c>
@@ -22561,7 +22563,7 @@
         <v>1897</v>
       </c>
     </row>
-    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="63" t="s">
         <v>93</v>
       </c>
@@ -22655,7 +22657,7 @@
         <v>1850</v>
       </c>
     </row>
-    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="64" t="s">
         <v>95</v>
       </c>
@@ -22702,7 +22704,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="64" t="s">
         <v>96</v>
       </c>
@@ -22749,7 +22751,7 @@
         <v>1851</v>
       </c>
     </row>
-    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="64" t="s">
         <v>97</v>
       </c>
@@ -22796,7 +22798,7 @@
         <v>1852</v>
       </c>
     </row>
-    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="64" t="s">
         <v>98</v>
       </c>
@@ -22843,7 +22845,7 @@
         <v>1853</v>
       </c>
     </row>
-    <row r="84" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="64" t="s">
         <v>99</v>
       </c>
@@ -22890,7 +22892,7 @@
         <v>1854</v>
       </c>
     </row>
-    <row r="85" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="64" t="s">
         <v>440</v>
       </c>
@@ -22937,7 +22939,7 @@
         <v>1899</v>
       </c>
     </row>
-    <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="64" t="s">
         <v>449</v>
       </c>
@@ -22984,7 +22986,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="64" t="s">
         <v>100</v>
       </c>
@@ -23031,7 +23033,7 @@
         <v>1901</v>
       </c>
     </row>
-    <row r="88" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="64" t="s">
         <v>101</v>
       </c>
@@ -23078,7 +23080,7 @@
         <v>1855</v>
       </c>
     </row>
-    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="64" t="s">
         <v>472</v>
       </c>
@@ -23125,7 +23127,7 @@
         <v>1856</v>
       </c>
     </row>
-    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="64" t="s">
         <v>102</v>
       </c>
@@ -23172,7 +23174,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="91" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="64" t="s">
         <v>103</v>
       </c>
@@ -23219,7 +23221,7 @@
         <v>1858</v>
       </c>
     </row>
-    <row r="92" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="64" t="s">
         <v>104</v>
       </c>
@@ -23266,7 +23268,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="64" t="s">
         <v>105</v>
       </c>
@@ -23313,7 +23315,7 @@
         <v>1860</v>
       </c>
     </row>
-    <row r="94" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="64" t="s">
         <v>106</v>
       </c>
@@ -23360,7 +23362,7 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="95" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="64" t="s">
         <v>107</v>
       </c>
@@ -23407,7 +23409,7 @@
         <v>1862</v>
       </c>
     </row>
-    <row r="96" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="64" t="s">
         <v>108</v>
       </c>
@@ -23454,7 +23456,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="97" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="64" t="s">
         <v>108</v>
       </c>
@@ -23522,13 +23524,7 @@
       <c r="O99" s="51"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O97">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Overlake Internal Medicine"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:O97"/>
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1"/>
     <hyperlink ref="K26" r:id="rId2"/>
@@ -23635,8 +23631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23647,12 +23643,12 @@
     <col min="4" max="4" width="10.140625" style="66" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="66" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.85546875" style="66" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" style="66" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="66" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="22.7109375" style="66" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="38.140625" style="66" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="19" style="66" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="57.28515625" style="66" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="66" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="66" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" style="66" customWidth="1"/>
+    <col min="10" max="10" width="38.140625" style="66" customWidth="1"/>
+    <col min="11" max="11" width="19" style="66" customWidth="1"/>
+    <col min="12" max="12" width="57.28515625" style="66" customWidth="1"/>
     <col min="13" max="13" width="11" style="66" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="32.42578125" style="66" customWidth="1"/>
     <col min="15" max="15" width="20.42578125" style="66" customWidth="1"/>
@@ -23717,7 +23713,7 @@
       <c r="B2" s="66" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="67">
+      <c r="C2" s="76">
         <v>19498</v>
       </c>
       <c r="D2" s="66" t="s">
@@ -23741,11 +23737,14 @@
       <c r="J2" s="66" t="s">
         <v>166</v>
       </c>
-      <c r="K2" s="68" t="s">
+      <c r="K2" s="67" t="s">
         <v>605</v>
       </c>
       <c r="L2" s="66" t="s">
         <v>1377</v>
+      </c>
+      <c r="M2" s="66">
+        <v>1</v>
       </c>
       <c r="N2" s="63" t="s">
         <v>93</v>
@@ -23764,7 +23763,7 @@
       <c r="B3" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="67">
+      <c r="C3" s="76">
         <v>31417</v>
       </c>
       <c r="D3" s="66" t="s">
@@ -23793,6 +23792,9 @@
       </c>
       <c r="L3" s="66" t="s">
         <v>1378</v>
+      </c>
+      <c r="M3" s="66">
+        <v>1</v>
       </c>
       <c r="N3" s="64" t="s">
         <v>94</v>
@@ -23811,7 +23813,7 @@
       <c r="B4" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="67">
+      <c r="C4" s="76">
         <v>35843</v>
       </c>
       <c r="D4" s="66" t="s">
@@ -23840,6 +23842,9 @@
       </c>
       <c r="L4" s="66" t="s">
         <v>1379</v>
+      </c>
+      <c r="M4" s="66">
+        <v>1</v>
       </c>
       <c r="N4" s="64" t="s">
         <v>95</v>
@@ -23858,7 +23863,7 @@
       <c r="B5" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="67">
+      <c r="C5" s="76">
         <v>32061</v>
       </c>
       <c r="D5" s="66" t="s">
@@ -23887,6 +23892,9 @@
       </c>
       <c r="L5" s="66" t="s">
         <v>1380</v>
+      </c>
+      <c r="M5" s="66">
+        <v>1</v>
       </c>
       <c r="N5" s="64" t="s">
         <v>96</v>
@@ -23905,7 +23913,7 @@
       <c r="B6" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="67">
+      <c r="C6" s="76">
         <v>22683</v>
       </c>
       <c r="D6" s="66" t="s">
@@ -23934,6 +23942,9 @@
       </c>
       <c r="L6" s="66" t="s">
         <v>1381</v>
+      </c>
+      <c r="M6" s="66">
+        <v>1</v>
       </c>
       <c r="N6" s="64" t="s">
         <v>97</v>
@@ -23952,7 +23963,7 @@
       <c r="B7" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="67">
+      <c r="C7" s="76">
         <v>27165</v>
       </c>
       <c r="D7" s="66" t="s">
@@ -23981,6 +23992,9 @@
       </c>
       <c r="L7" s="66" t="s">
         <v>1382</v>
+      </c>
+      <c r="M7" s="66">
+        <v>1</v>
       </c>
       <c r="N7" s="64" t="s">
         <v>98</v>
@@ -23999,7 +24013,7 @@
       <c r="B8" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="67">
+      <c r="C8" s="76">
         <v>33688</v>
       </c>
       <c r="D8" s="66" t="s">
@@ -24028,6 +24042,9 @@
       </c>
       <c r="L8" s="66" t="s">
         <v>1383</v>
+      </c>
+      <c r="M8" s="66">
+        <v>1</v>
       </c>
       <c r="N8" s="64" t="s">
         <v>99</v>
@@ -24046,7 +24063,7 @@
       <c r="B9" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="67">
+      <c r="C9" s="76">
         <v>33865</v>
       </c>
       <c r="D9" s="66" t="s">
@@ -24075,6 +24092,9 @@
       </c>
       <c r="L9" s="66" t="s">
         <v>1384</v>
+      </c>
+      <c r="M9" s="66">
+        <v>1</v>
       </c>
       <c r="N9" s="64" t="s">
         <v>440</v>
@@ -24093,7 +24113,7 @@
       <c r="B10" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="67">
+      <c r="C10" s="76">
         <v>25781</v>
       </c>
       <c r="D10" s="66" t="s">
@@ -24122,6 +24142,9 @@
       </c>
       <c r="L10" s="66" t="s">
         <v>1386</v>
+      </c>
+      <c r="M10" s="66">
+        <v>1</v>
       </c>
       <c r="N10" s="64" t="s">
         <v>449</v>
@@ -24140,7 +24163,7 @@
       <c r="B11" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="67">
+      <c r="C11" s="76">
         <v>31227</v>
       </c>
       <c r="D11" s="66" t="s">
@@ -24169,6 +24192,9 @@
       </c>
       <c r="L11" s="66" t="s">
         <v>1388</v>
+      </c>
+      <c r="M11" s="66">
+        <v>1</v>
       </c>
       <c r="N11" s="64" t="s">
         <v>100</v>
@@ -24187,7 +24213,7 @@
       <c r="B12" s="66" t="s">
         <v>546</v>
       </c>
-      <c r="C12" s="67">
+      <c r="C12" s="76">
         <v>22228</v>
       </c>
       <c r="D12" s="66" t="s">
@@ -24216,6 +24242,9 @@
       </c>
       <c r="L12" s="66" t="s">
         <v>1389</v>
+      </c>
+      <c r="M12" s="66">
+        <v>1</v>
       </c>
       <c r="N12" s="64" t="s">
         <v>101</v>
@@ -24234,7 +24263,7 @@
       <c r="B13" s="66" t="s">
         <v>553</v>
       </c>
-      <c r="C13" s="67">
+      <c r="C13" s="76">
         <v>21354</v>
       </c>
       <c r="D13" s="66" t="s">
@@ -24263,6 +24292,9 @@
       </c>
       <c r="L13" s="66" t="s">
         <v>1390</v>
+      </c>
+      <c r="M13" s="66">
+        <v>1</v>
       </c>
       <c r="N13" s="64" t="s">
         <v>472</v>
@@ -24281,7 +24313,7 @@
       <c r="B14" s="66" t="s">
         <v>554</v>
       </c>
-      <c r="C14" s="67">
+      <c r="C14" s="76">
         <v>39646</v>
       </c>
       <c r="D14" s="66" t="s">
@@ -24310,6 +24342,9 @@
       </c>
       <c r="L14" s="66" t="s">
         <v>1391</v>
+      </c>
+      <c r="M14" s="66">
+        <v>1</v>
       </c>
       <c r="N14" s="64" t="s">
         <v>102</v>
@@ -24328,7 +24363,7 @@
       <c r="B15" s="66" t="s">
         <v>556</v>
       </c>
-      <c r="C15" s="67">
+      <c r="C15" s="76">
         <v>30822</v>
       </c>
       <c r="D15" s="66" t="s">
@@ -24357,6 +24392,9 @@
       </c>
       <c r="L15" s="66" t="s">
         <v>1392</v>
+      </c>
+      <c r="M15" s="66">
+        <v>1</v>
       </c>
       <c r="N15" s="64" t="s">
         <v>103</v>
@@ -24375,7 +24413,7 @@
       <c r="B16" s="66" t="s">
         <v>558</v>
       </c>
-      <c r="C16" s="67">
+      <c r="C16" s="76">
         <v>29658</v>
       </c>
       <c r="D16" s="66" t="s">
@@ -24404,6 +24442,9 @@
       </c>
       <c r="L16" s="66" t="s">
         <v>1393</v>
+      </c>
+      <c r="M16" s="66">
+        <v>1</v>
       </c>
       <c r="N16" s="64" t="s">
         <v>104</v>
@@ -24422,7 +24463,7 @@
       <c r="B17" s="66" t="s">
         <v>560</v>
       </c>
-      <c r="C17" s="67">
+      <c r="C17" s="76">
         <v>27213</v>
       </c>
       <c r="D17" s="66" t="s">
@@ -24451,6 +24492,9 @@
       </c>
       <c r="L17" s="66" t="s">
         <v>1394</v>
+      </c>
+      <c r="M17" s="66">
+        <v>1</v>
       </c>
       <c r="N17" s="64" t="s">
         <v>105</v>
@@ -24469,7 +24513,7 @@
       <c r="B18" s="66" t="s">
         <v>562</v>
       </c>
-      <c r="C18" s="67">
+      <c r="C18" s="76">
         <v>39707</v>
       </c>
       <c r="D18" s="66" t="s">
@@ -24498,6 +24542,9 @@
       </c>
       <c r="L18" s="66" t="s">
         <v>1395</v>
+      </c>
+      <c r="M18" s="66">
+        <v>1</v>
       </c>
       <c r="N18" s="64" t="s">
         <v>106</v>
@@ -24516,7 +24563,7 @@
       <c r="B19" s="66" t="s">
         <v>564</v>
       </c>
-      <c r="C19" s="67">
+      <c r="C19" s="76">
         <v>30622</v>
       </c>
       <c r="D19" s="66" t="s">
@@ -24545,6 +24592,9 @@
       </c>
       <c r="L19" s="66" t="s">
         <v>1396</v>
+      </c>
+      <c r="M19" s="66">
+        <v>1</v>
       </c>
       <c r="N19" s="64" t="s">
         <v>107</v>
@@ -24563,7 +24613,7 @@
       <c r="B20" s="66" t="s">
         <v>566</v>
       </c>
-      <c r="C20" s="67">
+      <c r="C20" s="76">
         <v>31074</v>
       </c>
       <c r="D20" s="66" t="s">
@@ -24592,6 +24642,9 @@
       </c>
       <c r="L20" s="66" t="s">
         <v>1397</v>
+      </c>
+      <c r="M20" s="66">
+        <v>1</v>
       </c>
       <c r="N20" s="64" t="s">
         <v>108</v>
@@ -24610,7 +24663,7 @@
       <c r="B21" s="66" t="s">
         <v>568</v>
       </c>
-      <c r="C21" s="67">
+      <c r="C21" s="76">
         <v>15521</v>
       </c>
       <c r="D21" s="66" t="s">
@@ -24639,6 +24692,9 @@
       </c>
       <c r="L21" s="66" t="s">
         <v>1398</v>
+      </c>
+      <c r="M21" s="66">
+        <v>1</v>
       </c>
       <c r="N21" s="63" t="s">
         <v>93</v>
@@ -24657,7 +24713,7 @@
       <c r="B22" s="66" t="s">
         <v>570</v>
       </c>
-      <c r="C22" s="67">
+      <c r="C22" s="76">
         <v>22156</v>
       </c>
       <c r="D22" s="66" t="s">
@@ -24686,6 +24742,9 @@
       </c>
       <c r="L22" s="66" t="s">
         <v>1399</v>
+      </c>
+      <c r="M22" s="66">
+        <v>1</v>
       </c>
       <c r="N22" s="64" t="s">
         <v>94</v>
@@ -24704,7 +24763,7 @@
       <c r="B23" s="66" t="s">
         <v>572</v>
       </c>
-      <c r="C23" s="67">
+      <c r="C23" s="76">
         <v>32561</v>
       </c>
       <c r="D23" s="66" t="s">
@@ -24733,6 +24792,9 @@
       </c>
       <c r="L23" s="66" t="s">
         <v>1400</v>
+      </c>
+      <c r="M23" s="66">
+        <v>1</v>
       </c>
       <c r="N23" s="64" t="s">
         <v>95</v>
@@ -24751,7 +24813,7 @@
       <c r="B24" s="66" t="s">
         <v>573</v>
       </c>
-      <c r="C24" s="67">
+      <c r="C24" s="76">
         <v>16656</v>
       </c>
       <c r="D24" s="66" t="s">
@@ -24780,6 +24842,9 @@
       </c>
       <c r="L24" s="66" t="s">
         <v>1401</v>
+      </c>
+      <c r="M24" s="66">
+        <v>1</v>
       </c>
       <c r="N24" s="64" t="s">
         <v>96</v>
@@ -24798,7 +24863,7 @@
       <c r="B25" s="66" t="s">
         <v>575</v>
       </c>
-      <c r="C25" s="67">
+      <c r="C25" s="76">
         <v>28473</v>
       </c>
       <c r="D25" s="66" t="s">
@@ -24827,6 +24892,9 @@
       </c>
       <c r="L25" s="66" t="s">
         <v>1402</v>
+      </c>
+      <c r="M25" s="66">
+        <v>1</v>
       </c>
       <c r="N25" s="64" t="s">
         <v>97</v>
@@ -24845,7 +24913,7 @@
       <c r="B26" s="66" t="s">
         <v>577</v>
       </c>
-      <c r="C26" s="67">
+      <c r="C26" s="76">
         <v>12405</v>
       </c>
       <c r="D26" s="66" t="s">
@@ -24874,6 +24942,9 @@
       </c>
       <c r="L26" s="66" t="s">
         <v>1403</v>
+      </c>
+      <c r="M26" s="66">
+        <v>1</v>
       </c>
       <c r="N26" s="64" t="s">
         <v>98</v>
@@ -24892,7 +24963,7 @@
       <c r="B27" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="67">
+      <c r="C27" s="76">
         <v>38397</v>
       </c>
       <c r="D27" s="66" t="s">
@@ -24921,6 +24992,9 @@
       </c>
       <c r="L27" s="66" t="s">
         <v>1404</v>
+      </c>
+      <c r="M27" s="66">
+        <v>1</v>
       </c>
       <c r="N27" s="64" t="s">
         <v>99</v>
@@ -24939,7 +25013,7 @@
       <c r="B28" s="66" t="s">
         <v>612</v>
       </c>
-      <c r="C28" s="67">
+      <c r="C28" s="76">
         <v>28929</v>
       </c>
       <c r="D28" s="66" t="s">
@@ -24965,6 +25039,12 @@
       </c>
       <c r="K28" s="66" t="s">
         <v>615</v>
+      </c>
+      <c r="L28" s="66" t="s">
+        <v>1404</v>
+      </c>
+      <c r="M28" s="66">
+        <v>1</v>
       </c>
       <c r="N28" s="64" t="s">
         <v>440</v>
@@ -24983,7 +25063,7 @@
       <c r="B29" s="66" t="s">
         <v>617</v>
       </c>
-      <c r="C29" s="67">
+      <c r="C29" s="76">
         <v>30461</v>
       </c>
       <c r="D29" s="66" t="s">
@@ -25012,6 +25092,9 @@
       </c>
       <c r="L29" s="66" t="s">
         <v>1405</v>
+      </c>
+      <c r="M29" s="66">
+        <v>1</v>
       </c>
       <c r="N29" s="64" t="s">
         <v>449</v>
@@ -25030,7 +25113,7 @@
       <c r="B30" s="66" t="s">
         <v>621</v>
       </c>
-      <c r="C30" s="67">
+      <c r="C30" s="76">
         <v>20391</v>
       </c>
       <c r="D30" s="66" t="s">
@@ -25059,6 +25142,9 @@
       </c>
       <c r="L30" s="66" t="s">
         <v>1406</v>
+      </c>
+      <c r="M30" s="66">
+        <v>1</v>
       </c>
       <c r="N30" s="64" t="s">
         <v>100</v>
@@ -25077,7 +25163,7 @@
       <c r="B31" s="66" t="s">
         <v>625</v>
       </c>
-      <c r="C31" s="67">
+      <c r="C31" s="76">
         <v>18525</v>
       </c>
       <c r="D31" s="66" t="s">
@@ -25106,6 +25192,9 @@
       </c>
       <c r="L31" s="66" t="s">
         <v>1407</v>
+      </c>
+      <c r="M31" s="66">
+        <v>1</v>
       </c>
       <c r="N31" s="64" t="s">
         <v>101</v>
@@ -25124,7 +25213,7 @@
       <c r="B32" s="66" t="s">
         <v>629</v>
       </c>
-      <c r="C32" s="67">
+      <c r="C32" s="76">
         <v>32581</v>
       </c>
       <c r="D32" s="66" t="s">
@@ -25153,6 +25242,9 @@
       </c>
       <c r="L32" s="66" t="s">
         <v>1408</v>
+      </c>
+      <c r="M32" s="66">
+        <v>1</v>
       </c>
       <c r="N32" s="64" t="s">
         <v>472</v>
@@ -25171,7 +25263,7 @@
       <c r="B33" s="66" t="s">
         <v>155</v>
       </c>
-      <c r="C33" s="67">
+      <c r="C33" s="76">
         <v>29980</v>
       </c>
       <c r="D33" s="66" t="s">
@@ -25200,6 +25292,9 @@
       </c>
       <c r="L33" s="66" t="s">
         <v>1409</v>
+      </c>
+      <c r="M33" s="66">
+        <v>1</v>
       </c>
       <c r="N33" s="64" t="s">
         <v>102</v>
@@ -25218,7 +25313,7 @@
       <c r="B34" s="66" t="s">
         <v>636</v>
       </c>
-      <c r="C34" s="67">
+      <c r="C34" s="76">
         <v>31363</v>
       </c>
       <c r="D34" s="66" t="s">
@@ -25247,6 +25342,9 @@
       </c>
       <c r="L34" s="66" t="s">
         <v>1410</v>
+      </c>
+      <c r="M34" s="66">
+        <v>1</v>
       </c>
       <c r="N34" s="64" t="s">
         <v>103</v>
@@ -25265,7 +25363,7 @@
       <c r="B35" s="66" t="s">
         <v>639</v>
       </c>
-      <c r="C35" s="67">
+      <c r="C35" s="76">
         <v>30177</v>
       </c>
       <c r="D35" s="66" t="s">
@@ -25294,6 +25392,9 @@
       </c>
       <c r="L35" s="66" t="s">
         <v>1411</v>
+      </c>
+      <c r="M35" s="66">
+        <v>1</v>
       </c>
       <c r="N35" s="64" t="s">
         <v>104</v>
@@ -25312,7 +25413,7 @@
       <c r="B36" s="66" t="s">
         <v>643</v>
       </c>
-      <c r="C36" s="67">
+      <c r="C36" s="76">
         <v>31825</v>
       </c>
       <c r="D36" s="66" t="s">
@@ -25341,6 +25442,9 @@
       </c>
       <c r="L36" s="66" t="s">
         <v>1412</v>
+      </c>
+      <c r="M36" s="66">
+        <v>1</v>
       </c>
       <c r="N36" s="64" t="s">
         <v>105</v>
@@ -25359,7 +25463,7 @@
       <c r="B37" s="66" t="s">
         <v>646</v>
       </c>
-      <c r="C37" s="67">
+      <c r="C37" s="76">
         <v>31575</v>
       </c>
       <c r="D37" s="66" t="s">
@@ -25388,6 +25492,9 @@
       </c>
       <c r="L37" s="66" t="s">
         <v>1413</v>
+      </c>
+      <c r="M37" s="66">
+        <v>1</v>
       </c>
       <c r="N37" s="64" t="s">
         <v>106</v>
@@ -26359,7 +26466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add email column for patient
20726 - Upload data fix
</commit_message>
<xml_diff>
--- a/src/main/resources/OCP.xlsx
+++ b/src/main/resources/OCP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OCP\ocp-test-data\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4921" uniqueCount="1908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4922" uniqueCount="1909">
   <si>
     <t>First Name</t>
   </si>
@@ -5786,6 +5786,9 @@
   </si>
   <si>
     <t>organizaiton</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
@@ -23629,10 +23632,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K37"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23653,10 +23656,11 @@
     <col min="14" max="14" width="32.42578125" style="66" customWidth="1"/>
     <col min="15" max="15" width="20.42578125" style="66" customWidth="1"/>
     <col min="16" max="16" width="20.42578125" style="66" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="66"/>
+    <col min="17" max="17" width="30.5703125" style="66" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="66"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
@@ -23705,8 +23709,11 @@
       <c r="P1" s="66" t="s">
         <v>1770</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="66" t="s">
+        <v>1908</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="66" t="s">
         <v>164</v>
       </c>
@@ -23755,8 +23762,12 @@
       <c r="P2" s="61" t="s">
         <v>1790</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="66" t="str">
+        <f>CONCATENATE(A2, ".", B2, "@ocpmail.com")</f>
+        <v>Seymour.Patients@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
         <v>41</v>
       </c>
@@ -23805,8 +23816,12 @@
       <c r="P3" s="66" t="s">
         <v>1791</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="66" t="str">
+        <f t="shared" ref="Q3:Q37" si="0">CONCATENATE(A3, ".", B3, "@ocpmail.com")</f>
+        <v>Sally.Share@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="66" t="s">
         <v>11</v>
       </c>
@@ -23855,8 +23870,12 @@
       <c r="P4" s="66" t="s">
         <v>1792</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Andreas.Lockman@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="66" t="s">
         <v>13</v>
       </c>
@@ -23905,8 +23924,12 @@
       <c r="P5" s="66" t="s">
         <v>1793</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Asa.Greenfelder@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="66" t="s">
         <v>15</v>
       </c>
@@ -23955,8 +23978,12 @@
       <c r="P6" s="66" t="s">
         <v>1794</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Beth.Hermiston@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="66" t="s">
         <v>17</v>
       </c>
@@ -24005,8 +24032,12 @@
       <c r="P7" s="66" t="s">
         <v>1795</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Blair.Maggio@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="66" t="s">
         <v>19</v>
       </c>
@@ -24055,8 +24086,12 @@
       <c r="P8" s="66" t="s">
         <v>1796</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Buck.Cronin@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="66" t="s">
         <v>21</v>
       </c>
@@ -24105,8 +24140,12 @@
       <c r="P9" s="66" t="s">
         <v>1797</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Deja.Ledner@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="66" t="s">
         <v>1385</v>
       </c>
@@ -24155,8 +24194,12 @@
       <c r="P10" s="66" t="s">
         <v>1798</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Edie.Weber@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="66" t="s">
         <v>1387</v>
       </c>
@@ -24205,8 +24248,12 @@
       <c r="P11" s="66" t="s">
         <v>1799</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Eleanor.Jacobs@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="66" t="s">
         <v>545</v>
       </c>
@@ -24255,8 +24302,12 @@
       <c r="P12" s="66" t="s">
         <v>1800</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Bernardo.Espinosa@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="66" t="s">
         <v>552</v>
       </c>
@@ -24305,8 +24356,12 @@
       <c r="P13" s="66" t="s">
         <v>1801</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q13" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Brent.Weimann@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="66" t="s">
         <v>159</v>
       </c>
@@ -24355,8 +24410,12 @@
       <c r="P14" s="66" t="s">
         <v>1802</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q14" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Brian.Armstrong@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="66" t="s">
         <v>555</v>
       </c>
@@ -24405,8 +24464,12 @@
       <c r="P15" s="66" t="s">
         <v>1803</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q15" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Catina.Smitham@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="66" t="s">
         <v>557</v>
       </c>
@@ -24455,8 +24518,12 @@
       <c r="P16" s="66" t="s">
         <v>1804</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Felicia.Breitenberg@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="66" t="s">
         <v>559</v>
       </c>
@@ -24505,8 +24572,12 @@
       <c r="P17" s="66" t="s">
         <v>1805</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Fredda.Greenholt@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="66" t="s">
         <v>561</v>
       </c>
@@ -24555,8 +24626,12 @@
       <c r="P18" s="66" t="s">
         <v>1806</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Kimberli.Murphy@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="66" t="s">
         <v>563</v>
       </c>
@@ -24605,8 +24680,12 @@
       <c r="P19" s="66" t="s">
         <v>1807</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Kindra.Davis@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="66" t="s">
         <v>565</v>
       </c>
@@ -24655,8 +24734,12 @@
       <c r="P20" s="66" t="s">
         <v>1808</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q20" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Leida.Miller@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="66" t="s">
         <v>567</v>
       </c>
@@ -24705,8 +24788,12 @@
       <c r="P21" s="66" t="s">
         <v>1809</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q21" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Linnea.Dooley@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="66" t="s">
         <v>569</v>
       </c>
@@ -24755,8 +24842,12 @@
       <c r="P22" s="66" t="s">
         <v>1810</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q22" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Milan.Beer@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="66" t="s">
         <v>571</v>
       </c>
@@ -24805,8 +24896,12 @@
       <c r="P23" s="66" t="s">
         <v>1811</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q23" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Penelope.Orn@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="66" t="s">
         <v>156</v>
       </c>
@@ -24855,8 +24950,12 @@
       <c r="P24" s="66" t="s">
         <v>1812</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q24" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Ryan.Stark@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="66" t="s">
         <v>574</v>
       </c>
@@ -24905,8 +25004,12 @@
       <c r="P25" s="66" t="s">
         <v>1813</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q25" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Sofia.Salinas@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="66" t="s">
         <v>576</v>
       </c>
@@ -24955,8 +25058,12 @@
       <c r="P26" s="66" t="s">
         <v>1814</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q26" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Sylvie.Steuber@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="66" t="s">
         <v>578</v>
       </c>
@@ -25005,8 +25112,12 @@
       <c r="P27" s="66" t="s">
         <v>1815</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q27" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Yung.Jacobs@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="66" t="s">
         <v>83</v>
       </c>
@@ -25055,8 +25166,12 @@
       <c r="P28" s="66" t="s">
         <v>1816</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q28" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Mark.Warner@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="66" t="s">
         <v>616</v>
       </c>
@@ -25105,8 +25220,12 @@
       <c r="P29" s="66" t="s">
         <v>1817</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q29" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Marcy.Grey@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="66" t="s">
         <v>620</v>
       </c>
@@ -25155,8 +25274,12 @@
       <c r="P30" s="66" t="s">
         <v>1818</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q30" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>William.Harry@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="66" t="s">
         <v>624</v>
       </c>
@@ -25205,8 +25328,12 @@
       <c r="P31" s="66" t="s">
         <v>1819</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q31" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Antoino.Ramos@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="66" t="s">
         <v>157</v>
       </c>
@@ -25255,8 +25382,12 @@
       <c r="P32" s="66" t="s">
         <v>1820</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q32" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Mary.Moore@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="66" t="s">
         <v>632</v>
       </c>
@@ -25305,8 +25436,12 @@
       <c r="P33" s="66" t="s">
         <v>1821</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q33" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Bob.Moses@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="66" t="s">
         <v>635</v>
       </c>
@@ -25355,8 +25490,12 @@
       <c r="P34" s="66" t="s">
         <v>1822</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q34" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Chet .Baker@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="66" t="s">
         <v>162</v>
       </c>
@@ -25405,8 +25544,12 @@
       <c r="P35" s="66" t="s">
         <v>1823</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q35" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Stephen.Wright@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="66" t="s">
         <v>642</v>
       </c>
@@ -25455,8 +25598,12 @@
       <c r="P36" s="66" t="s">
         <v>1824</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q36" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Brenda.Parker@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="66" t="s">
         <v>1769</v>
       </c>
@@ -25505,11 +25652,15 @@
       <c r="P37" s="66" t="s">
         <v>1825</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q37" s="66" t="str">
+        <f t="shared" si="0"/>
+        <v>Johnny.Jesus@ocpmail.com</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N38" s="64"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N39" s="64"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct date of birth column of related person
20941 - Update Demo site with Latest code and Test Data
</commit_message>
<xml_diff>
--- a/src/main/resources/OCP.xlsx
+++ b/src/main/resources/OCP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8895" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8895" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Organizations" sheetId="5" r:id="rId1"/>
@@ -5774,7 +5774,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -5908,6 +5908,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
@@ -16984,7 +16985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D106" sqref="D106"/>
     </sheetView>
@@ -23859,8 +23860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23939,7 +23940,7 @@
       <c r="D2" s="29" t="s">
         <v>1373</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E2" s="57">
         <v>32249</v>
       </c>
       <c r="F2" s="29" t="s">
@@ -23992,7 +23993,7 @@
       <c r="D3" s="29" t="s">
         <v>1374</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="57">
         <v>33733</v>
       </c>
       <c r="F3" s="29" t="s">
@@ -24045,7 +24046,7 @@
       <c r="D4" s="29" t="s">
         <v>1375</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="57">
         <v>30995</v>
       </c>
       <c r="F4" s="29" t="s">
@@ -24098,7 +24099,7 @@
       <c r="D5" s="29" t="s">
         <v>1376</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="57">
         <v>27750</v>
       </c>
       <c r="F5" s="29" t="s">
@@ -24151,7 +24152,7 @@
       <c r="D6" s="29" t="s">
         <v>1373</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="57">
         <v>34879</v>
       </c>
       <c r="F6" s="29" t="s">
@@ -24204,7 +24205,7 @@
       <c r="D7" s="29" t="s">
         <v>1374</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="57">
         <v>18549</v>
       </c>
       <c r="F7" s="29" t="s">
@@ -24257,7 +24258,7 @@
       <c r="D8" s="29" t="s">
         <v>1377</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="57">
         <v>32421</v>
       </c>
       <c r="F8" s="29" t="s">
@@ -24310,7 +24311,7 @@
       <c r="D9" s="29" t="s">
         <v>1373</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="57">
         <v>22213</v>
       </c>
       <c r="F9" s="29" t="s">
@@ -24363,7 +24364,7 @@
       <c r="D10" s="29" t="s">
         <v>1374</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="57">
         <v>16657</v>
       </c>
       <c r="F10" s="29" t="s">
@@ -24416,7 +24417,7 @@
       <c r="D11" s="29" t="s">
         <v>1377</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="57">
         <v>31720</v>
       </c>
       <c r="F11" s="29" t="s">
@@ -24469,7 +24470,7 @@
       <c r="D12" s="29" t="s">
         <v>1378</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="57">
         <v>30045</v>
       </c>
       <c r="F12" s="29" t="s">
@@ -24522,7 +24523,7 @@
       <c r="D13" s="29" t="s">
         <v>1379</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="57">
         <v>28345</v>
       </c>
       <c r="F13" s="29" t="s">

</xml_diff>

<commit_message>
Fix Related Persons issue and add EMail for Related Persons
</commit_message>
<xml_diff>
--- a/src/main/resources/OCP.xlsx
+++ b/src/main/resources/OCP.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\c2s-ws\ocp-ws\ocp-test-data\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\intellij-workspaces\ocp\ocp-test-data\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8895" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8892" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Organizations" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Patient Related Persons'!$A$1:$N$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Practitioners!$A$1:$O$96</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4459" uniqueCount="1847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4472" uniqueCount="1860">
   <si>
     <t>First Name</t>
   </si>
@@ -5592,12 +5592,51 @@
   </si>
   <si>
     <t>j.emmett.cm</t>
+  </si>
+  <si>
+    <t>Contact-Email</t>
+  </si>
+  <si>
+    <t>Deandelo.Francis@mailinator.com</t>
+  </si>
+  <si>
+    <t>Jimena.Bean@mailinator.com</t>
+  </si>
+  <si>
+    <t>Ashlee.Gill@mailinator.com</t>
+  </si>
+  <si>
+    <t>Stephen.Fletcher@mailinator.com</t>
+  </si>
+  <si>
+    <t>Gunnar.Glass@mailinator.com</t>
+  </si>
+  <si>
+    <t>Reed.Miles@mailinator.com</t>
+  </si>
+  <si>
+    <t>Wilson.Horton@mailinator.com</t>
+  </si>
+  <si>
+    <t>Finnegan.Small@mailinator.com</t>
+  </si>
+  <si>
+    <t>Carla.Pace@mailinator.com</t>
+  </si>
+  <si>
+    <t>Branden.Kirk@mailinator.com</t>
+  </si>
+  <si>
+    <t>Edie.Weber@mailinator.com</t>
+  </si>
+  <si>
+    <t>Eleanor.Jacobs@mailinator.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="00000"/>
@@ -5774,7 +5813,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -5909,6 +5948,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="4" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
@@ -7013,18 +7053,18 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="26" style="10" customWidth="1"/>
     <col min="7" max="7" width="41" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="10"/>
+    <col min="8" max="8" width="51.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>263</v>
       </c>
@@ -7053,7 +7093,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>73</v>
       </c>
@@ -7082,7 +7122,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>74</v>
       </c>
@@ -7111,7 +7151,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>75</v>
       </c>
@@ -7140,7 +7180,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>76</v>
       </c>
@@ -7169,7 +7209,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>77</v>
       </c>
@@ -7198,7 +7238,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>78</v>
       </c>
@@ -7227,7 +7267,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>79</v>
       </c>
@@ -7256,7 +7296,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>351</v>
       </c>
@@ -7285,7 +7325,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>360</v>
       </c>
@@ -7314,7 +7354,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>80</v>
       </c>
@@ -7343,7 +7383,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>81</v>
       </c>
@@ -7372,7 +7412,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>383</v>
       </c>
@@ -7401,7 +7441,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>82</v>
       </c>
@@ -7430,7 +7470,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>83</v>
       </c>
@@ -7459,7 +7499,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>84</v>
       </c>
@@ -7488,7 +7528,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>85</v>
       </c>
@@ -7517,7 +7557,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>86</v>
       </c>
@@ -7546,7 +7586,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>87</v>
       </c>
@@ -7575,7 +7615,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>88</v>
       </c>
@@ -7604,7 +7644,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="54" t="s">
         <v>1837</v>
       </c>
@@ -7633,7 +7673,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="54" t="s">
         <v>1828</v>
       </c>
@@ -7662,7 +7702,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="54" t="s">
         <v>1812</v>
       </c>
@@ -7691,7 +7731,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>1820</v>
       </c>
@@ -7737,22 +7777,22 @@
       <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="10"/>
+    <col min="11" max="16384" width="8.88671875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>58</v>
       </c>
@@ -7784,7 +7824,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>73</v>
       </c>
@@ -7816,7 +7856,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>73</v>
       </c>
@@ -7848,7 +7888,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>73</v>
       </c>
@@ -7880,7 +7920,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>73</v>
       </c>
@@ -7912,7 +7952,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
         <v>73</v>
       </c>
@@ -7944,7 +7984,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>74</v>
       </c>
@@ -7976,7 +8016,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
         <v>74</v>
       </c>
@@ -8008,7 +8048,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
         <v>74</v>
       </c>
@@ -8040,7 +8080,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
         <v>74</v>
       </c>
@@ -8072,7 +8112,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>74</v>
       </c>
@@ -8104,7 +8144,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
         <v>75</v>
       </c>
@@ -8136,7 +8176,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
         <v>75</v>
       </c>
@@ -8168,7 +8208,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>75</v>
       </c>
@@ -8200,7 +8240,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
         <v>75</v>
       </c>
@@ -8232,7 +8272,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
         <v>75</v>
       </c>
@@ -8264,7 +8304,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
         <v>76</v>
       </c>
@@ -8296,7 +8336,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>76</v>
       </c>
@@ -8328,7 +8368,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
         <v>76</v>
       </c>
@@ -8360,7 +8400,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>76</v>
       </c>
@@ -8392,7 +8432,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21" t="s">
         <v>76</v>
       </c>
@@ -8424,7 +8464,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
         <v>77</v>
       </c>
@@ -8456,7 +8496,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
         <v>77</v>
       </c>
@@ -8488,7 +8528,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="21" t="s">
         <v>77</v>
       </c>
@@ -8520,7 +8560,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
         <v>77</v>
       </c>
@@ -8552,7 +8592,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
         <v>77</v>
       </c>
@@ -8584,7 +8624,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
         <v>78</v>
       </c>
@@ -8616,7 +8656,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
         <v>78</v>
       </c>
@@ -8648,7 +8688,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
         <v>78</v>
       </c>
@@ -8680,7 +8720,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="21" t="s">
         <v>78</v>
       </c>
@@ -8712,7 +8752,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
         <v>78</v>
       </c>
@@ -8744,7 +8784,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="21" t="s">
         <v>79</v>
       </c>
@@ -8776,7 +8816,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
         <v>79</v>
       </c>
@@ -8808,7 +8848,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="21" t="s">
         <v>79</v>
       </c>
@@ -8840,7 +8880,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>79</v>
       </c>
@@ -8872,7 +8912,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="21" t="s">
         <v>79</v>
       </c>
@@ -8904,7 +8944,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
         <v>351</v>
       </c>
@@ -8936,7 +8976,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="21" t="s">
         <v>351</v>
       </c>
@@ -8968,7 +9008,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="21" t="s">
         <v>351</v>
       </c>
@@ -9000,7 +9040,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="21" t="s">
         <v>351</v>
       </c>
@@ -9032,7 +9072,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="21" t="s">
         <v>351</v>
       </c>
@@ -9064,7 +9104,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="21" t="s">
         <v>360</v>
       </c>
@@ -9096,7 +9136,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="21" t="s">
         <v>360</v>
       </c>
@@ -9128,7 +9168,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="21" t="s">
         <v>360</v>
       </c>
@@ -9160,7 +9200,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="21" t="s">
         <v>360</v>
       </c>
@@ -9192,7 +9232,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="21" t="s">
         <v>360</v>
       </c>
@@ -9224,7 +9264,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="21" t="s">
         <v>80</v>
       </c>
@@ -9256,7 +9296,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="21" t="s">
         <v>80</v>
       </c>
@@ -9288,7 +9328,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="21" t="s">
         <v>80</v>
       </c>
@@ -9320,7 +9360,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="21" t="s">
         <v>80</v>
       </c>
@@ -9352,7 +9392,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="21" t="s">
         <v>80</v>
       </c>
@@ -9384,7 +9424,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="21" t="s">
         <v>81</v>
       </c>
@@ -9416,7 +9456,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="21" t="s">
         <v>81</v>
       </c>
@@ -9448,7 +9488,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="21" t="s">
         <v>81</v>
       </c>
@@ -9480,7 +9520,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="21" t="s">
         <v>81</v>
       </c>
@@ -9512,7 +9552,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="21" t="s">
         <v>81</v>
       </c>
@@ -9544,7 +9584,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="21" t="s">
         <v>383</v>
       </c>
@@ -9576,7 +9616,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="21" t="s">
         <v>383</v>
       </c>
@@ -9608,7 +9648,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="21" t="s">
         <v>383</v>
       </c>
@@ -9640,7 +9680,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="21" t="s">
         <v>383</v>
       </c>
@@ -9672,7 +9712,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="21" t="s">
         <v>383</v>
       </c>
@@ -9704,7 +9744,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="21" t="s">
         <v>82</v>
       </c>
@@ -9736,7 +9776,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="21" t="s">
         <v>82</v>
       </c>
@@ -9768,7 +9808,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="21" t="s">
         <v>82</v>
       </c>
@@ -9800,7 +9840,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="21" t="s">
         <v>82</v>
       </c>
@@ -9832,7 +9872,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="21" t="s">
         <v>82</v>
       </c>
@@ -9864,7 +9904,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="21" t="s">
         <v>83</v>
       </c>
@@ -9896,7 +9936,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="21" t="s">
         <v>83</v>
       </c>
@@ -9928,7 +9968,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="21" t="s">
         <v>83</v>
       </c>
@@ -9960,7 +10000,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="70" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="21" t="s">
         <v>83</v>
       </c>
@@ -9992,7 +10032,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="71" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="21" t="s">
         <v>83</v>
       </c>
@@ -10024,7 +10064,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="21" t="s">
         <v>84</v>
       </c>
@@ -10056,7 +10096,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="21" t="s">
         <v>84</v>
       </c>
@@ -10088,7 +10128,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="21" t="s">
         <v>84</v>
       </c>
@@ -10120,7 +10160,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="21" t="s">
         <v>84</v>
       </c>
@@ -10152,7 +10192,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="76" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="21" t="s">
         <v>84</v>
       </c>
@@ -10184,7 +10224,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="77" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="21" t="s">
         <v>85</v>
       </c>
@@ -10216,7 +10256,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="78" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="21" t="s">
         <v>85</v>
       </c>
@@ -10248,7 +10288,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="79" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="21" t="s">
         <v>85</v>
       </c>
@@ -10280,7 +10320,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="80" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="21" t="s">
         <v>85</v>
       </c>
@@ -10312,7 +10352,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="21" t="s">
         <v>85</v>
       </c>
@@ -10344,7 +10384,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="82" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="21" t="s">
         <v>86</v>
       </c>
@@ -10376,7 +10416,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="83" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="21" t="s">
         <v>86</v>
       </c>
@@ -10408,7 +10448,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="84" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="21" t="s">
         <v>86</v>
       </c>
@@ -10440,7 +10480,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="85" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="21" t="s">
         <v>86</v>
       </c>
@@ -10472,7 +10512,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="86" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="21" t="s">
         <v>86</v>
       </c>
@@ -10504,7 +10544,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="87" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="21" t="s">
         <v>87</v>
       </c>
@@ -10536,7 +10576,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="88" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="21" t="s">
         <v>87</v>
       </c>
@@ -10568,7 +10608,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="89" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="21" t="s">
         <v>87</v>
       </c>
@@ -10600,7 +10640,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="90" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="21" t="s">
         <v>87</v>
       </c>
@@ -10632,7 +10672,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="91" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="21" t="s">
         <v>87</v>
       </c>
@@ -10664,7 +10704,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="92" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="21" t="s">
         <v>88</v>
       </c>
@@ -10696,7 +10736,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="93" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="21" t="s">
         <v>88</v>
       </c>
@@ -10728,7 +10768,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="94" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="21" t="s">
         <v>88</v>
       </c>
@@ -10760,7 +10800,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="95" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="21" t="s">
         <v>88</v>
       </c>
@@ -10792,7 +10832,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="96" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="21" t="s">
         <v>88</v>
       </c>
@@ -10824,7 +10864,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="97" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="54" t="s">
         <v>1837</v>
       </c>
@@ -10856,7 +10896,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
         <v>1812</v>
       </c>
@@ -10888,7 +10928,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
         <v>1820</v>
       </c>
@@ -10920,7 +10960,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="100" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="54" t="s">
         <v>1828</v>
       </c>
@@ -10970,20 +11010,20 @@
       <selection pane="bottomLeft" activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="10"/>
+    <col min="1" max="1" width="30.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>58</v>
       </c>
@@ -11009,7 +11049,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>383</v>
       </c>
@@ -11035,7 +11075,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>383</v>
       </c>
@@ -11061,7 +11101,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>383</v>
       </c>
@@ -11087,7 +11127,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>383</v>
       </c>
@@ -11113,7 +11153,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>383</v>
       </c>
@@ -11139,7 +11179,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>74</v>
       </c>
@@ -11165,7 +11205,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>74</v>
       </c>
@@ -11191,7 +11231,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>74</v>
       </c>
@@ -11217,7 +11257,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>74</v>
       </c>
@@ -11243,7 +11283,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>74</v>
       </c>
@@ -11269,7 +11309,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>75</v>
       </c>
@@ -11295,7 +11335,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>75</v>
       </c>
@@ -11321,7 +11361,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>75</v>
       </c>
@@ -11347,7 +11387,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>75</v>
       </c>
@@ -11373,7 +11413,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>75</v>
       </c>
@@ -11399,7 +11439,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>76</v>
       </c>
@@ -11425,7 +11465,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>76</v>
       </c>
@@ -11451,7 +11491,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>76</v>
       </c>
@@ -11477,7 +11517,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>76</v>
       </c>
@@ -11503,7 +11543,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>76</v>
       </c>
@@ -11529,7 +11569,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>77</v>
       </c>
@@ -11555,7 +11595,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>77</v>
       </c>
@@ -11581,7 +11621,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>77</v>
       </c>
@@ -11607,7 +11647,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>77</v>
       </c>
@@ -11633,7 +11673,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>77</v>
       </c>
@@ -11659,7 +11699,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>78</v>
       </c>
@@ -11685,7 +11725,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>78</v>
       </c>
@@ -11711,7 +11751,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>78</v>
       </c>
@@ -11737,7 +11777,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>78</v>
       </c>
@@ -11763,7 +11803,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>78</v>
       </c>
@@ -11789,7 +11829,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>79</v>
       </c>
@@ -11815,7 +11855,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>79</v>
       </c>
@@ -11841,7 +11881,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>79</v>
       </c>
@@ -11867,7 +11907,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>79</v>
       </c>
@@ -11893,7 +11933,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>79</v>
       </c>
@@ -11919,7 +11959,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>351</v>
       </c>
@@ -11945,7 +11985,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>351</v>
       </c>
@@ -11971,7 +12011,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
         <v>351</v>
       </c>
@@ -11997,7 +12037,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>351</v>
       </c>
@@ -12023,7 +12063,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>351</v>
       </c>
@@ -12049,7 +12089,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>360</v>
       </c>
@@ -12075,7 +12115,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>360</v>
       </c>
@@ -12101,7 +12141,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>360</v>
       </c>
@@ -12127,7 +12167,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>360</v>
       </c>
@@ -12153,7 +12193,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
         <v>360</v>
       </c>
@@ -12179,7 +12219,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>80</v>
       </c>
@@ -12205,7 +12245,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>80</v>
       </c>
@@ -12231,7 +12271,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>80</v>
       </c>
@@ -12257,7 +12297,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>80</v>
       </c>
@@ -12283,7 +12323,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>80</v>
       </c>
@@ -12309,7 +12349,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>81</v>
       </c>
@@ -12335,7 +12375,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>81</v>
       </c>
@@ -12361,7 +12401,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>81</v>
       </c>
@@ -12387,7 +12427,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
         <v>81</v>
       </c>
@@ -12413,7 +12453,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
         <v>81</v>
       </c>
@@ -12439,7 +12479,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
         <v>383</v>
       </c>
@@ -12465,7 +12505,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
         <v>383</v>
       </c>
@@ -12491,7 +12531,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
         <v>383</v>
       </c>
@@ -12517,7 +12557,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
         <v>383</v>
       </c>
@@ -12543,7 +12583,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
         <v>383</v>
       </c>
@@ -12569,7 +12609,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
         <v>82</v>
       </c>
@@ -12595,7 +12635,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>82</v>
       </c>
@@ -12621,7 +12661,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
         <v>82</v>
       </c>
@@ -12647,7 +12687,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
         <v>82</v>
       </c>
@@ -12673,7 +12713,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="10" t="s">
         <v>82</v>
       </c>
@@ -12699,7 +12739,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="10" t="s">
         <v>83</v>
       </c>
@@ -12725,7 +12765,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="10" t="s">
         <v>83</v>
       </c>
@@ -12751,7 +12791,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="10" t="s">
         <v>83</v>
       </c>
@@ -12777,7 +12817,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="10" t="s">
         <v>83</v>
       </c>
@@ -12803,7 +12843,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="10" t="s">
         <v>83</v>
       </c>
@@ -12829,7 +12869,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="10" t="s">
         <v>84</v>
       </c>
@@ -12855,7 +12895,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="10" t="s">
         <v>84</v>
       </c>
@@ -12881,7 +12921,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="10" t="s">
         <v>84</v>
       </c>
@@ -12907,7 +12947,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
         <v>84</v>
       </c>
@@ -12933,7 +12973,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="10" t="s">
         <v>84</v>
       </c>
@@ -12959,7 +12999,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="10" t="s">
         <v>85</v>
       </c>
@@ -12985,7 +13025,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="10" t="s">
         <v>85</v>
       </c>
@@ -13011,7 +13051,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="10" t="s">
         <v>85</v>
       </c>
@@ -13037,7 +13077,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="10" t="s">
         <v>85</v>
       </c>
@@ -13063,7 +13103,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="10" t="s">
         <v>85</v>
       </c>
@@ -13089,7 +13129,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="10" t="s">
         <v>86</v>
       </c>
@@ -13115,7 +13155,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="10" t="s">
         <v>86</v>
       </c>
@@ -13141,7 +13181,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="10" t="s">
         <v>86</v>
       </c>
@@ -13165,7 +13205,7 @@
       </c>
       <c r="H84" s="10"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="10" t="s">
         <v>86</v>
       </c>
@@ -13191,7 +13231,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="10" t="s">
         <v>86</v>
       </c>
@@ -13217,7 +13257,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="10" t="s">
         <v>87</v>
       </c>
@@ -13243,7 +13283,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="10" t="s">
         <v>87</v>
       </c>
@@ -13269,7 +13309,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="10" t="s">
         <v>87</v>
       </c>
@@ -13295,7 +13335,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="10" t="s">
         <v>87</v>
       </c>
@@ -13321,7 +13361,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="10" t="s">
         <v>87</v>
       </c>
@@ -13347,7 +13387,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="10" t="s">
         <v>88</v>
       </c>
@@ -13373,7 +13413,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="10" t="s">
         <v>88</v>
       </c>
@@ -13399,7 +13439,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="10" t="s">
         <v>88</v>
       </c>
@@ -13425,7 +13465,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="10" t="s">
         <v>88</v>
       </c>
@@ -13451,7 +13491,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="10" t="s">
         <v>1812</v>
       </c>
@@ -13564,27 +13604,27 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" style="7" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5546875" style="7" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="7"/>
+    <col min="15" max="15" width="18.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>58</v>
       </c>
@@ -13631,7 +13671,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>73</v>
       </c>
@@ -13675,7 +13715,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>73</v>
       </c>
@@ -13719,7 +13759,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>73</v>
       </c>
@@ -13763,7 +13803,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>73</v>
       </c>
@@ -13807,7 +13847,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>73</v>
       </c>
@@ -13851,7 +13891,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>73</v>
       </c>
@@ -13895,7 +13935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>74</v>
       </c>
@@ -13939,7 +13979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>74</v>
       </c>
@@ -13983,7 +14023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>74</v>
       </c>
@@ -14027,7 +14067,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>74</v>
       </c>
@@ -14071,7 +14111,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>74</v>
       </c>
@@ -14115,7 +14155,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>75</v>
       </c>
@@ -14159,7 +14199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>75</v>
       </c>
@@ -14203,7 +14243,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>75</v>
       </c>
@@ -14247,7 +14287,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>75</v>
       </c>
@@ -14291,7 +14331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>251</v>
       </c>
@@ -14335,7 +14375,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>251</v>
       </c>
@@ -14379,7 +14419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>251</v>
       </c>
@@ -14423,7 +14463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>251</v>
       </c>
@@ -14467,7 +14507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>251</v>
       </c>
@@ -14511,7 +14551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>251</v>
       </c>
@@ -14555,7 +14595,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>77</v>
       </c>
@@ -14599,7 +14639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>78</v>
       </c>
@@ -14643,7 +14683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>78</v>
       </c>
@@ -14687,7 +14727,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>78</v>
       </c>
@@ -14731,7 +14771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>78</v>
       </c>
@@ -14775,7 +14815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>78</v>
       </c>
@@ -14819,7 +14859,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>78</v>
       </c>
@@ -14863,7 +14903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>79</v>
       </c>
@@ -14907,7 +14947,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>79</v>
       </c>
@@ -14951,7 +14991,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>79</v>
       </c>
@@ -14995,7 +15035,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>79</v>
       </c>
@@ -15039,7 +15079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>79</v>
       </c>
@@ -15083,7 +15123,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>79</v>
       </c>
@@ -15127,7 +15167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>81</v>
       </c>
@@ -15171,7 +15211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>81</v>
       </c>
@@ -15215,7 +15255,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>81</v>
       </c>
@@ -15259,7 +15299,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>81</v>
       </c>
@@ -15303,7 +15343,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>81</v>
       </c>
@@ -15347,7 +15387,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>81</v>
       </c>
@@ -15391,7 +15431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>85</v>
       </c>
@@ -15435,7 +15475,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>85</v>
       </c>
@@ -15479,7 +15519,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>85</v>
       </c>
@@ -15523,7 +15563,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>85</v>
       </c>
@@ -15567,7 +15607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>85</v>
       </c>
@@ -15611,7 +15651,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>85</v>
       </c>
@@ -15655,7 +15695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>86</v>
       </c>
@@ -15699,7 +15739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>86</v>
       </c>
@@ -15743,7 +15783,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>86</v>
       </c>
@@ -15787,7 +15827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>86</v>
       </c>
@@ -15831,7 +15871,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>86</v>
       </c>
@@ -15875,7 +15915,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>86</v>
       </c>
@@ -15919,7 +15959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>87</v>
       </c>
@@ -15963,7 +16003,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>87</v>
       </c>
@@ -16007,7 +16047,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>87</v>
       </c>
@@ -16051,7 +16091,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>87</v>
       </c>
@@ -16095,7 +16135,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>87</v>
       </c>
@@ -16139,7 +16179,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>87</v>
       </c>
@@ -16183,7 +16223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>88</v>
       </c>
@@ -16227,7 +16267,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
         <v>88</v>
       </c>
@@ -16271,7 +16311,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
         <v>88</v>
       </c>
@@ -16315,7 +16355,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>88</v>
       </c>
@@ -16359,7 +16399,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
         <v>88</v>
       </c>
@@ -16403,7 +16443,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
         <v>88</v>
       </c>
@@ -16447,7 +16487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>383</v>
       </c>
@@ -16491,7 +16531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
         <v>383</v>
       </c>
@@ -16535,7 +16575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
         <v>383</v>
       </c>
@@ -16579,7 +16619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
         <v>383</v>
       </c>
@@ -16623,7 +16663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
         <v>383</v>
       </c>
@@ -16667,7 +16707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
         <v>383</v>
       </c>
@@ -16711,7 +16751,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
         <v>351</v>
       </c>
@@ -16755,7 +16795,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
         <v>360</v>
       </c>
@@ -16799,7 +16839,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
         <v>360</v>
       </c>
@@ -16843,7 +16883,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
         <v>360</v>
       </c>
@@ -16887,7 +16927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" s="7" t="s">
         <v>383</v>
       </c>
@@ -16931,7 +16971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
         <v>80</v>
       </c>
@@ -16990,28 +17030,28 @@
       <selection pane="bottomLeft" activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="66" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="19" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" style="19" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="19" customWidth="1"/>
     <col min="4" max="4" width="17" style="19" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="19" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="34" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="34" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" style="34" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" style="34" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="34" customWidth="1"/>
+    <col min="8" max="8" width="5.5546875" style="34" customWidth="1"/>
     <col min="9" max="9" width="6" style="34" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" style="19" customWidth="1"/>
-    <col min="11" max="11" width="48.85546875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" style="19" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" style="19" customWidth="1"/>
+    <col min="11" max="11" width="48.88671875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" style="19" customWidth="1"/>
     <col min="13" max="13" width="12" style="6" customWidth="1"/>
-    <col min="14" max="14" width="36.140625" style="19" customWidth="1"/>
-    <col min="15" max="15" width="23.28515625" style="19" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="19" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="19"/>
+    <col min="14" max="14" width="36.109375" style="19" customWidth="1"/>
+    <col min="15" max="15" width="23.33203125" style="19" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" style="19" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="41" t="s">
         <v>58</v>
       </c>
@@ -17058,7 +17098,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
         <v>73</v>
       </c>
@@ -17105,7 +17145,7 @@
         <v>1636</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="43" t="s">
         <v>74</v>
       </c>
@@ -17152,7 +17192,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="43" t="s">
         <v>75</v>
       </c>
@@ -17199,7 +17239,7 @@
         <v>1638</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="43" t="s">
         <v>76</v>
       </c>
@@ -17246,7 +17286,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="43" t="s">
         <v>77</v>
       </c>
@@ -17293,7 +17333,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="43" t="s">
         <v>78</v>
       </c>
@@ -17340,7 +17380,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="43" t="s">
         <v>79</v>
       </c>
@@ -17387,7 +17427,7 @@
         <v>1642</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="43" t="s">
         <v>351</v>
       </c>
@@ -17434,7 +17474,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="43" t="s">
         <v>360</v>
       </c>
@@ -17481,7 +17521,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="43" t="s">
         <v>80</v>
       </c>
@@ -17528,7 +17568,7 @@
         <v>1645</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="43" t="s">
         <v>81</v>
       </c>
@@ -17575,7 +17615,7 @@
         <v>1654</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="43" t="s">
         <v>383</v>
       </c>
@@ -17622,7 +17662,7 @@
         <v>1646</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="43" t="s">
         <v>82</v>
       </c>
@@ -17669,7 +17709,7 @@
         <v>1647</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="43" t="s">
         <v>83</v>
       </c>
@@ -17716,7 +17756,7 @@
         <v>1648</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="43" t="s">
         <v>84</v>
       </c>
@@ -17763,7 +17803,7 @@
         <v>1649</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="43" t="s">
         <v>85</v>
       </c>
@@ -17810,7 +17850,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="43" t="s">
         <v>86</v>
       </c>
@@ -17857,7 +17897,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="43" t="s">
         <v>87</v>
       </c>
@@ -17904,7 +17944,7 @@
         <v>1652</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="43" t="s">
         <v>88</v>
       </c>
@@ -17951,7 +17991,7 @@
         <v>1653</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="42" t="s">
         <v>73</v>
       </c>
@@ -17998,7 +18038,7 @@
         <v>1691</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="43" t="s">
         <v>74</v>
       </c>
@@ -18045,7 +18085,7 @@
         <v>1692</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="43" t="s">
         <v>75</v>
       </c>
@@ -18092,7 +18132,7 @@
         <v>1693</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="43" t="s">
         <v>76</v>
       </c>
@@ -18139,7 +18179,7 @@
         <v>1694</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="43" t="s">
         <v>77</v>
       </c>
@@ -18186,7 +18226,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="43" t="s">
         <v>78</v>
       </c>
@@ -18233,7 +18273,7 @@
         <v>1696</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="43" t="s">
         <v>79</v>
       </c>
@@ -18280,7 +18320,7 @@
         <v>1697</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="43" t="s">
         <v>351</v>
       </c>
@@ -18327,7 +18367,7 @@
         <v>1698</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="43" t="s">
         <v>360</v>
       </c>
@@ -18374,7 +18414,7 @@
         <v>1699</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="43" t="s">
         <v>80</v>
       </c>
@@ -18421,7 +18461,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="43" t="s">
         <v>81</v>
       </c>
@@ -18468,7 +18508,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="43" t="s">
         <v>383</v>
       </c>
@@ -18515,7 +18555,7 @@
         <v>1702</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="43" t="s">
         <v>82</v>
       </c>
@@ -18562,7 +18602,7 @@
         <v>1703</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="43" t="s">
         <v>83</v>
       </c>
@@ -18609,7 +18649,7 @@
         <v>1704</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="43" t="s">
         <v>84</v>
       </c>
@@ -18656,7 +18696,7 @@
         <v>1705</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="43" t="s">
         <v>85</v>
       </c>
@@ -18703,7 +18743,7 @@
         <v>1706</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="43" t="s">
         <v>86</v>
       </c>
@@ -18750,7 +18790,7 @@
         <v>1707</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="43" t="s">
         <v>87</v>
       </c>
@@ -18797,7 +18837,7 @@
         <v>1708</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="43" t="s">
         <v>88</v>
       </c>
@@ -18844,7 +18884,7 @@
         <v>1709</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="42" t="s">
         <v>73</v>
       </c>
@@ -18891,7 +18931,7 @@
         <v>1729</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="43" t="s">
         <v>75</v>
       </c>
@@ -18938,7 +18978,7 @@
         <v>1730</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="43" t="s">
         <v>76</v>
       </c>
@@ -18985,7 +19025,7 @@
         <v>1731</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="43" t="s">
         <v>77</v>
       </c>
@@ -19032,7 +19072,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="43" t="s">
         <v>78</v>
       </c>
@@ -19079,7 +19119,7 @@
         <v>1733</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="43" t="s">
         <v>79</v>
       </c>
@@ -19126,7 +19166,7 @@
         <v>1734</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="43" t="s">
         <v>351</v>
       </c>
@@ -19173,7 +19213,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="43" t="s">
         <v>360</v>
       </c>
@@ -19220,7 +19260,7 @@
         <v>1735</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="43" t="s">
         <v>80</v>
       </c>
@@ -19267,7 +19307,7 @@
         <v>1736</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="43" t="s">
         <v>81</v>
       </c>
@@ -19314,7 +19354,7 @@
         <v>1737</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="43" t="s">
         <v>383</v>
       </c>
@@ -19361,7 +19401,7 @@
         <v>1738</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="43" t="s">
         <v>82</v>
       </c>
@@ -19408,7 +19448,7 @@
         <v>1739</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="43" t="s">
         <v>83</v>
       </c>
@@ -19455,7 +19495,7 @@
         <v>1740</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="43" t="s">
         <v>84</v>
       </c>
@@ -19502,7 +19542,7 @@
         <v>1741</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="43" t="s">
         <v>85</v>
       </c>
@@ -19549,7 +19589,7 @@
         <v>1742</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="43" t="s">
         <v>86</v>
       </c>
@@ -19596,7 +19636,7 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="43" t="s">
         <v>87</v>
       </c>
@@ -19643,7 +19683,7 @@
         <v>1744</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="43" t="s">
         <v>88</v>
       </c>
@@ -19690,7 +19730,7 @@
         <v>1745</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="42" t="s">
         <v>73</v>
       </c>
@@ -19737,7 +19777,7 @@
         <v>1746</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="43" t="s">
         <v>74</v>
       </c>
@@ -19784,7 +19824,7 @@
         <v>1747</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="43" t="s">
         <v>75</v>
       </c>
@@ -19831,7 +19871,7 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="43" t="s">
         <v>76</v>
       </c>
@@ -19878,7 +19918,7 @@
         <v>1748</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="43" t="s">
         <v>77</v>
       </c>
@@ -19925,7 +19965,7 @@
         <v>1749</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="43" t="s">
         <v>78</v>
       </c>
@@ -19972,7 +20012,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="43" t="s">
         <v>79</v>
       </c>
@@ -20019,7 +20059,7 @@
         <v>1751</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" s="43" t="s">
         <v>351</v>
       </c>
@@ -20066,7 +20106,7 @@
         <v>1752</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="43" t="s">
         <v>360</v>
       </c>
@@ -20113,7 +20153,7 @@
         <v>1712</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="43" t="s">
         <v>80</v>
       </c>
@@ -20160,7 +20200,7 @@
         <v>1713</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="43" t="s">
         <v>81</v>
       </c>
@@ -20207,7 +20247,7 @@
         <v>1753</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="43" t="s">
         <v>383</v>
       </c>
@@ -20254,7 +20294,7 @@
         <v>1754</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" s="43" t="s">
         <v>82</v>
       </c>
@@ -20301,7 +20341,7 @@
         <v>1755</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="43" t="s">
         <v>83</v>
       </c>
@@ -20348,7 +20388,7 @@
         <v>1756</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="43" t="s">
         <v>84</v>
       </c>
@@ -20395,7 +20435,7 @@
         <v>1757</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="43" t="s">
         <v>85</v>
       </c>
@@ -20442,7 +20482,7 @@
         <v>1758</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="43" t="s">
         <v>86</v>
       </c>
@@ -20489,7 +20529,7 @@
         <v>1759</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" s="43" t="s">
         <v>87</v>
       </c>
@@ -20536,7 +20576,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="43" t="s">
         <v>88</v>
       </c>
@@ -20583,7 +20623,7 @@
         <v>1761</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="42" t="s">
         <v>73</v>
       </c>
@@ -20630,7 +20670,7 @@
         <v>1714</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" s="43" t="s">
         <v>74</v>
       </c>
@@ -20677,7 +20717,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="43" t="s">
         <v>75</v>
       </c>
@@ -20724,7 +20764,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" s="43" t="s">
         <v>76</v>
       </c>
@@ -20771,7 +20811,7 @@
         <v>1716</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" s="43" t="s">
         <v>77</v>
       </c>
@@ -20818,7 +20858,7 @@
         <v>1717</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" s="43" t="s">
         <v>78</v>
       </c>
@@ -20865,7 +20905,7 @@
         <v>1718</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" s="43" t="s">
         <v>79</v>
       </c>
@@ -20912,7 +20952,7 @@
         <v>1719</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" s="43" t="s">
         <v>351</v>
       </c>
@@ -20959,7 +20999,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" s="43" t="s">
         <v>360</v>
       </c>
@@ -21006,7 +21046,7 @@
         <v>1764</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" s="43" t="s">
         <v>80</v>
       </c>
@@ -21053,7 +21093,7 @@
         <v>1765</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" s="43" t="s">
         <v>81</v>
       </c>
@@ -21100,7 +21140,7 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" s="43" t="s">
         <v>383</v>
       </c>
@@ -21147,7 +21187,7 @@
         <v>1721</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" s="43" t="s">
         <v>82</v>
       </c>
@@ -21194,7 +21234,7 @@
         <v>1722</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" s="43" t="s">
         <v>83</v>
       </c>
@@ -21241,7 +21281,7 @@
         <v>1723</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" s="43" t="s">
         <v>84</v>
       </c>
@@ -21288,7 +21328,7 @@
         <v>1724</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" s="43" t="s">
         <v>85</v>
       </c>
@@ -21335,7 +21375,7 @@
         <v>1725</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" s="43" t="s">
         <v>86</v>
       </c>
@@ -21382,7 +21422,7 @@
         <v>1726</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" s="43" t="s">
         <v>87</v>
       </c>
@@ -21429,7 +21469,7 @@
         <v>1727</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" s="43" t="s">
         <v>88</v>
       </c>
@@ -21476,7 +21516,7 @@
         <v>1766</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" s="43" t="s">
         <v>88</v>
       </c>
@@ -21523,7 +21563,7 @@
         <v>1728</v>
       </c>
     </row>
-    <row r="97" spans="1:15" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="54" t="s">
         <v>1828</v>
       </c>
@@ -21570,7 +21610,7 @@
         <v>1811</v>
       </c>
     </row>
-    <row r="98" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
         <v>1820</v>
       </c>
@@ -21617,7 +21657,7 @@
         <v>1836</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" s="40" t="s">
         <v>1812</v>
       </c>
@@ -21664,7 +21704,7 @@
         <v>1846</v>
       </c>
     </row>
-    <row r="100" spans="1:15" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="54" t="s">
         <v>1837</v>
       </c>
@@ -21822,29 +21862,29 @@
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="45" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="45" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="45" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" style="45" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" style="45" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="45" customWidth="1"/>
-    <col min="9" max="9" width="22.7109375" style="45" customWidth="1"/>
-    <col min="10" max="10" width="38.140625" style="45" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" style="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" style="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="45" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.88671875" style="45" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="45" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="45" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" style="45" customWidth="1"/>
+    <col min="10" max="10" width="38.109375" style="45" customWidth="1"/>
     <col min="11" max="11" width="19" style="45" customWidth="1"/>
-    <col min="12" max="12" width="57.28515625" style="45" customWidth="1"/>
+    <col min="12" max="12" width="57.33203125" style="45" customWidth="1"/>
     <col min="13" max="13" width="11" style="45" customWidth="1"/>
-    <col min="14" max="14" width="32.42578125" style="45" customWidth="1"/>
-    <col min="15" max="15" width="20.42578125" style="45" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" style="45" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.5703125" style="45" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="45"/>
+    <col min="14" max="14" width="32.44140625" style="45" customWidth="1"/>
+    <col min="15" max="15" width="20.44140625" style="45" customWidth="1"/>
+    <col min="16" max="16" width="20.44140625" style="45" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.5546875" style="45" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
@@ -21897,7 +21937,7 @@
         <v>1767</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
         <v>144</v>
       </c>
@@ -21950,7 +21990,7 @@
         <v>1768</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="45" t="s">
         <v>41</v>
       </c>
@@ -22003,7 +22043,7 @@
         <v>1769</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="45" t="s">
         <v>11</v>
       </c>
@@ -22056,7 +22096,7 @@
         <v>1770</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="45" t="s">
         <v>13</v>
       </c>
@@ -22109,7 +22149,7 @@
         <v>1771</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="45" t="s">
         <v>15</v>
       </c>
@@ -22162,7 +22202,7 @@
         <v>1772</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="45" t="s">
         <v>17</v>
       </c>
@@ -22215,7 +22255,7 @@
         <v>1773</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="45" t="s">
         <v>19</v>
       </c>
@@ -22268,7 +22308,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="45" t="s">
         <v>21</v>
       </c>
@@ -22321,7 +22361,7 @@
         <v>1775</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="45" t="s">
         <v>1288</v>
       </c>
@@ -22374,7 +22414,7 @@
         <v>1776</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="45" t="s">
         <v>1290</v>
       </c>
@@ -22427,7 +22467,7 @@
         <v>1777</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="45" t="s">
         <v>456</v>
       </c>
@@ -22480,7 +22520,7 @@
         <v>1778</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="45" t="s">
         <v>463</v>
       </c>
@@ -22533,7 +22573,7 @@
         <v>1779</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="45" t="s">
         <v>139</v>
       </c>
@@ -22586,7 +22626,7 @@
         <v>1780</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="45" t="s">
         <v>466</v>
       </c>
@@ -22639,7 +22679,7 @@
         <v>1781</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="45" t="s">
         <v>468</v>
       </c>
@@ -22692,7 +22732,7 @@
         <v>1782</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="45" t="s">
         <v>470</v>
       </c>
@@ -22745,7 +22785,7 @@
         <v>1783</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="45" t="s">
         <v>472</v>
       </c>
@@ -22798,7 +22838,7 @@
         <v>1784</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="45" t="s">
         <v>474</v>
       </c>
@@ -22851,7 +22891,7 @@
         <v>1785</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="45" t="s">
         <v>476</v>
       </c>
@@ -22904,7 +22944,7 @@
         <v>1786</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="45" t="s">
         <v>478</v>
       </c>
@@ -22957,7 +22997,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="45" t="s">
         <v>480</v>
       </c>
@@ -23010,7 +23050,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="45" t="s">
         <v>482</v>
       </c>
@@ -23063,7 +23103,7 @@
         <v>1789</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="45" t="s">
         <v>136</v>
       </c>
@@ -23116,7 +23156,7 @@
         <v>1790</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="45" t="s">
         <v>485</v>
       </c>
@@ -23169,7 +23209,7 @@
         <v>1791</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="45" t="s">
         <v>487</v>
       </c>
@@ -23222,7 +23262,7 @@
         <v>1792</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="45" t="s">
         <v>489</v>
       </c>
@@ -23275,7 +23315,7 @@
         <v>1793</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="45" t="s">
         <v>63</v>
       </c>
@@ -23328,7 +23368,7 @@
         <v>1794</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="45" t="s">
         <v>527</v>
       </c>
@@ -23381,7 +23421,7 @@
         <v>1795</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="45" t="s">
         <v>531</v>
       </c>
@@ -23434,7 +23474,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="45" t="s">
         <v>535</v>
       </c>
@@ -23487,7 +23527,7 @@
         <v>1802</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="45" t="s">
         <v>137</v>
       </c>
@@ -23540,7 +23580,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="45" t="s">
         <v>543</v>
       </c>
@@ -23593,7 +23633,7 @@
         <v>1798</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="45" t="s">
         <v>546</v>
       </c>
@@ -23646,7 +23686,7 @@
         <v>1799</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="45" t="s">
         <v>142</v>
       </c>
@@ -23699,7 +23739,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="45" t="s">
         <v>553</v>
       </c>
@@ -23752,7 +23792,7 @@
         <v>1801</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="45" t="s">
         <v>1634</v>
       </c>
@@ -23805,10 +23845,10 @@
         <v>1803</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N38" s="43"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N39" s="43"/>
     </row>
   </sheetData>
@@ -23861,29 +23901,29 @@
   <dimension ref="A1:W24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E13"/>
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18" style="29" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" style="29" customWidth="1"/>
+    <col min="11" max="11" width="18" style="29" customWidth="1"/>
+    <col min="12" max="12" width="7.88671875" style="29" customWidth="1"/>
     <col min="13" max="13" width="11" style="29" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="3"/>
+    <col min="14" max="14" width="16.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
@@ -23926,8 +23966,11 @@
       <c r="N1" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="4" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>147</v>
       </c>
@@ -23970,7 +24013,9 @@
       <c r="N2" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="O2" s="29"/>
+      <c r="O2" s="58" t="s">
+        <v>1848</v>
+      </c>
       <c r="P2" s="29"/>
       <c r="Q2" s="29"/>
       <c r="R2" s="29"/>
@@ -23980,7 +24025,7 @@
       <c r="V2" s="29"/>
       <c r="W2" s="29"/>
     </row>
-    <row r="3" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>147</v>
       </c>
@@ -24023,7 +24068,9 @@
       <c r="N3" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="O3" s="29"/>
+      <c r="O3" s="58" t="s">
+        <v>1849</v>
+      </c>
       <c r="P3" s="29"/>
       <c r="Q3" s="29"/>
       <c r="R3" s="29"/>
@@ -24033,7 +24080,7 @@
       <c r="V3" s="29"/>
       <c r="W3" s="29"/>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>47</v>
       </c>
@@ -24076,7 +24123,9 @@
       <c r="N4" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="O4" s="29"/>
+      <c r="O4" s="58" t="s">
+        <v>1850</v>
+      </c>
       <c r="P4" s="29"/>
       <c r="Q4" s="29"/>
       <c r="R4" s="29"/>
@@ -24086,7 +24135,7 @@
       <c r="V4" s="29"/>
       <c r="W4" s="29"/>
     </row>
-    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>47</v>
       </c>
@@ -24129,7 +24178,9 @@
       <c r="N5" s="29" t="s">
         <v>191</v>
       </c>
-      <c r="O5" s="29"/>
+      <c r="O5" s="58" t="s">
+        <v>1851</v>
+      </c>
       <c r="P5" s="29"/>
       <c r="Q5" s="29"/>
       <c r="R5" s="29"/>
@@ -24139,7 +24190,7 @@
       <c r="V5" s="29"/>
       <c r="W5" s="29"/>
     </row>
-    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>48</v>
       </c>
@@ -24182,7 +24233,9 @@
       <c r="N6" s="29" t="s">
         <v>192</v>
       </c>
-      <c r="O6" s="29"/>
+      <c r="O6" s="58" t="s">
+        <v>1852</v>
+      </c>
       <c r="P6" s="29"/>
       <c r="Q6" s="29"/>
       <c r="R6" s="29"/>
@@ -24192,7 +24245,7 @@
       <c r="V6" s="29"/>
       <c r="W6" s="29"/>
     </row>
-    <row r="7" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>49</v>
       </c>
@@ -24235,7 +24288,9 @@
       <c r="N7" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="O7" s="29"/>
+      <c r="O7" s="58" t="s">
+        <v>1853</v>
+      </c>
       <c r="P7" s="29"/>
       <c r="Q7" s="29"/>
       <c r="R7" s="29"/>
@@ -24245,7 +24300,7 @@
       <c r="V7" s="29"/>
       <c r="W7" s="29"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>50</v>
       </c>
@@ -24288,7 +24343,9 @@
       <c r="N8" s="29" t="s">
         <v>187</v>
       </c>
-      <c r="O8" s="29"/>
+      <c r="O8" s="58" t="s">
+        <v>1854</v>
+      </c>
       <c r="P8" s="29"/>
       <c r="Q8" s="29"/>
       <c r="R8" s="29"/>
@@ -24298,7 +24355,7 @@
       <c r="V8" s="29"/>
       <c r="W8" s="29"/>
     </row>
-    <row r="9" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>51</v>
       </c>
@@ -24341,7 +24398,9 @@
       <c r="N9" s="29" t="s">
         <v>188</v>
       </c>
-      <c r="O9" s="29"/>
+      <c r="O9" s="58" t="s">
+        <v>1855</v>
+      </c>
       <c r="P9" s="29"/>
       <c r="Q9" s="29"/>
       <c r="R9" s="29"/>
@@ -24351,7 +24410,7 @@
       <c r="V9" s="29"/>
       <c r="W9" s="29"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>52</v>
       </c>
@@ -24394,7 +24453,9 @@
       <c r="N10" s="29" t="s">
         <v>189</v>
       </c>
-      <c r="O10" s="29"/>
+      <c r="O10" s="58" t="s">
+        <v>1856</v>
+      </c>
       <c r="P10" s="29"/>
       <c r="Q10" s="29"/>
       <c r="R10" s="29"/>
@@ -24404,7 +24465,7 @@
       <c r="V10" s="29"/>
       <c r="W10" s="29"/>
     </row>
-    <row r="11" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>53</v>
       </c>
@@ -24447,7 +24508,9 @@
       <c r="N11" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="O11" s="29"/>
+      <c r="O11" s="58" t="s">
+        <v>1857</v>
+      </c>
       <c r="P11" s="29"/>
       <c r="Q11" s="29"/>
       <c r="R11" s="29"/>
@@ -24457,7 +24520,7 @@
       <c r="V11" s="29"/>
       <c r="W11" s="29"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>54</v>
       </c>
@@ -24500,7 +24563,9 @@
       <c r="N12" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="O12" s="29"/>
+      <c r="O12" s="58" t="s">
+        <v>1858</v>
+      </c>
       <c r="P12" s="29"/>
       <c r="Q12" s="29"/>
       <c r="R12" s="29"/>
@@ -24510,7 +24575,7 @@
       <c r="V12" s="29"/>
       <c r="W12" s="29"/>
     </row>
-    <row r="13" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>55</v>
       </c>
@@ -24553,7 +24618,9 @@
       <c r="N13" s="29" t="s">
         <v>190</v>
       </c>
-      <c r="O13" s="29"/>
+      <c r="O13" s="58" t="s">
+        <v>1859</v>
+      </c>
       <c r="P13" s="29"/>
       <c r="Q13" s="29"/>
       <c r="R13" s="29"/>
@@ -24563,7 +24630,7 @@
       <c r="V13" s="29"/>
       <c r="W13" s="29"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="29"/>
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
@@ -24584,7 +24651,7 @@
       <c r="V14" s="29"/>
       <c r="W14" s="29"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
@@ -24605,7 +24672,7 @@
       <c r="V15" s="29"/>
       <c r="W15" s="29"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="29"/>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
@@ -24626,7 +24693,7 @@
       <c r="V16" s="29"/>
       <c r="W16" s="29"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="29"/>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
@@ -24647,7 +24714,7 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="29"/>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
@@ -24668,7 +24735,7 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="29"/>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
@@ -24688,7 +24755,7 @@
       <c r="V19" s="29"/>
       <c r="W19" s="29"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="29"/>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
@@ -24709,7 +24776,7 @@
       <c r="V20" s="29"/>
       <c r="W20" s="29"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="29"/>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
@@ -24730,7 +24797,7 @@
       <c r="V21" s="29"/>
       <c r="W21" s="29"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="29"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
@@ -24751,7 +24818,7 @@
       <c r="V22" s="29"/>
       <c r="W22" s="29"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="29"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
@@ -24772,7 +24839,7 @@
       <c r="V23" s="29"/>
       <c r="W23" s="29"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="29"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
@@ -24794,7 +24861,21 @@
       <c r="W24" s="29"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O2" r:id="rId1"/>
+    <hyperlink ref="O3" r:id="rId2"/>
+    <hyperlink ref="O4" r:id="rId3"/>
+    <hyperlink ref="O5" r:id="rId4"/>
+    <hyperlink ref="O6" r:id="rId5"/>
+    <hyperlink ref="O7" r:id="rId6"/>
+    <hyperlink ref="O8" r:id="rId7"/>
+    <hyperlink ref="O9" r:id="rId8"/>
+    <hyperlink ref="O10" r:id="rId9"/>
+    <hyperlink ref="O11" r:id="rId10"/>
+    <hyperlink ref="O12" r:id="rId11"/>
+    <hyperlink ref="O13" r:id="rId12"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove MES conference data
20941 - Update Demo site with Latest code and Test Data
</commit_message>
<xml_diff>
--- a/src/main/resources/OCP.xlsx
+++ b/src/main/resources/OCP.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\intellij-workspaces\ocp\ocp-test-data\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\c2s-ws\ocp-ws\ocp-test-data\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8892" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8892" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Organizations" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4472" uniqueCount="1860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4350" uniqueCount="1817">
   <si>
     <t>First Name</t>
   </si>
@@ -5463,135 +5463,6 @@
   </si>
   <si>
     <t>johnny.jesus@mailinator.com</t>
-  </si>
-  <si>
-    <t>Toledo</t>
-  </si>
-  <si>
-    <t>903 S. Telegraph, Ste. A</t>
-  </si>
-  <si>
-    <t>Monroe</t>
-  </si>
-  <si>
-    <t>MI</t>
-  </si>
-  <si>
-    <t>734-555-7200</t>
-  </si>
-  <si>
-    <t>Ellen</t>
-  </si>
-  <si>
-    <t>ellen.davis@mailinator.com</t>
-  </si>
-  <si>
-    <t>e.davis.cc</t>
-  </si>
-  <si>
-    <t>Substance Abuse Services, Inc</t>
-  </si>
-  <si>
-    <t>1916 N 12th St</t>
-  </si>
-  <si>
-    <t>SAS0001</t>
-  </si>
-  <si>
-    <t>Toledo Location</t>
-  </si>
-  <si>
-    <t>Methadone Maintenance Treatment Program (MMTP)</t>
-  </si>
-  <si>
-    <t>RESIDENTIAL SUB-ACUTE DETOXIFICATION (detox)</t>
-  </si>
-  <si>
-    <t>Drug and/or Alcohol Counselling</t>
-  </si>
-  <si>
-    <t>Rehabilitation</t>
-  </si>
-  <si>
-    <t>Monroe County Probation</t>
-  </si>
-  <si>
-    <t>125 E 2nd St</t>
-  </si>
-  <si>
-    <t>734-555-7100</t>
-  </si>
-  <si>
-    <t>Reagan</t>
-  </si>
-  <si>
-    <t>Probation Officer</t>
-  </si>
-  <si>
-    <t>daniel.reagan@mailenator.com</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>333 S. Grand Ave P.O. Box 30195</t>
-  </si>
-  <si>
-    <t>Michigan Department of Health and Human Services</t>
-  </si>
-  <si>
-    <t>Lansing</t>
-  </si>
-  <si>
-    <t>517-335-9030</t>
-  </si>
-  <si>
-    <t>419-555-6020</t>
-  </si>
-  <si>
-    <t>Jordon</t>
-  </si>
-  <si>
-    <t>Emmett</t>
-  </si>
-  <si>
-    <t>Addiction Psychiatry</t>
-  </si>
-  <si>
-    <t>jordon.emmett@mailenator.com</t>
-  </si>
-  <si>
-    <t>d.reagan.cm</t>
-  </si>
-  <si>
-    <t>Bay Creek Emergency Services</t>
-  </si>
-  <si>
-    <t>7157 Jackman Rd</t>
-  </si>
-  <si>
-    <t>Temperance</t>
-  </si>
-  <si>
-    <t>734-555-9779</t>
-  </si>
-  <si>
-    <t>Trace</t>
-  </si>
-  <si>
-    <t>Farooq</t>
-  </si>
-  <si>
-    <t>Emergency Medicine Physician</t>
-  </si>
-  <si>
-    <t>trace.farooq@mailenator.com</t>
-  </si>
-  <si>
-    <t>t.farooq.cm</t>
-  </si>
-  <si>
-    <t>j.emmett.cm</t>
   </si>
   <si>
     <t>Contact-Email</t>
@@ -5636,7 +5507,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="00000"/>
@@ -7050,7 +6921,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A21" sqref="A21:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7645,120 +7516,41 @@
       </c>
     </row>
     <row r="21" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="54" t="s">
-        <v>1837</v>
-      </c>
-      <c r="B21" s="56" t="s">
-        <v>1839</v>
-      </c>
-      <c r="C21" s="56" t="s">
-        <v>1838</v>
-      </c>
-      <c r="D21" s="56" t="s">
-        <v>1839</v>
-      </c>
-      <c r="E21" s="56" t="s">
-        <v>1807</v>
-      </c>
-      <c r="F21" s="56">
-        <v>48182</v>
-      </c>
-      <c r="G21" s="42" t="s">
-        <v>1840</v>
-      </c>
-      <c r="H21" s="54">
-        <v>237645898</v>
-      </c>
-      <c r="I21" s="54" t="s">
-        <v>56</v>
-      </c>
+      <c r="A21" s="54"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
     </row>
     <row r="22" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="54" t="s">
-        <v>1828</v>
-      </c>
-      <c r="B22" s="54" t="s">
-        <v>1829</v>
-      </c>
-      <c r="C22" s="54" t="s">
-        <v>1827</v>
-      </c>
-      <c r="D22" s="54" t="s">
-        <v>1829</v>
-      </c>
-      <c r="E22" s="54" t="s">
-        <v>1807</v>
-      </c>
-      <c r="F22" s="54">
-        <v>48909</v>
-      </c>
-      <c r="G22" s="54" t="s">
-        <v>1830</v>
-      </c>
-      <c r="H22" s="54">
-        <v>897651456</v>
-      </c>
-      <c r="I22" s="54" t="s">
-        <v>56</v>
-      </c>
+      <c r="A22" s="54"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
     </row>
     <row r="23" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="54" t="s">
-        <v>1812</v>
-      </c>
-      <c r="B23" s="54" t="s">
-        <v>1815</v>
-      </c>
-      <c r="C23" s="54" t="s">
-        <v>1813</v>
-      </c>
-      <c r="D23" s="54" t="s">
-        <v>1804</v>
-      </c>
-      <c r="E23" s="54" t="s">
-        <v>1427</v>
-      </c>
-      <c r="F23" s="54">
-        <v>43634</v>
-      </c>
-      <c r="G23" s="54" t="s">
-        <v>1831</v>
-      </c>
-      <c r="H23" s="54">
-        <v>987122345</v>
-      </c>
-      <c r="I23" s="54" t="s">
-        <v>56</v>
-      </c>
+      <c r="A23" s="54"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
-        <v>1820</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>1806</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>1821</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>1806</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>1807</v>
-      </c>
-      <c r="F24" s="10">
-        <v>48161</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>1822</v>
-      </c>
-      <c r="H24" s="10">
-        <v>8192818</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>56</v>
-      </c>
+      <c r="E24" s="6"/>
+      <c r="I24" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7773,8 +7565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView topLeftCell="A83" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97:XFD107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10865,132 +10657,48 @@
       </c>
     </row>
     <row r="97" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="54" t="s">
-        <v>1837</v>
-      </c>
-      <c r="B97" s="56" t="s">
-        <v>1839</v>
-      </c>
-      <c r="C97" s="56" t="s">
-        <v>1838</v>
-      </c>
-      <c r="D97" s="56" t="s">
-        <v>1839</v>
-      </c>
-      <c r="E97" s="56" t="s">
-        <v>1807</v>
-      </c>
-      <c r="F97" s="56">
-        <v>48182</v>
-      </c>
-      <c r="G97" s="42" t="s">
-        <v>1840</v>
-      </c>
-      <c r="H97" s="15" t="s">
-        <v>569</v>
-      </c>
-      <c r="I97" s="54">
-        <v>237645898</v>
-      </c>
-      <c r="J97" s="54" t="s">
-        <v>56</v>
-      </c>
+      <c r="A97" s="54"/>
+      <c r="B97" s="56"/>
+      <c r="C97" s="56"/>
+      <c r="D97" s="56"/>
+      <c r="E97" s="56"/>
+      <c r="F97" s="56"/>
+      <c r="G97" s="42"/>
+      <c r="H97" s="15"/>
+      <c r="I97" s="54"/>
+      <c r="J97" s="54"/>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A98" s="6" t="s">
-        <v>1812</v>
-      </c>
-      <c r="B98" s="10" t="s">
-        <v>1815</v>
-      </c>
-      <c r="C98" s="10" t="s">
-        <v>1813</v>
-      </c>
-      <c r="D98" s="10" t="s">
-        <v>1804</v>
-      </c>
-      <c r="E98" s="6" t="s">
-        <v>1427</v>
-      </c>
-      <c r="F98" s="10">
-        <v>43634</v>
-      </c>
-      <c r="G98" s="10" t="s">
-        <v>1808</v>
-      </c>
-      <c r="H98" s="15" t="s">
-        <v>569</v>
-      </c>
-      <c r="I98" s="6" t="s">
-        <v>1814</v>
-      </c>
-      <c r="J98" s="6" t="s">
-        <v>56</v>
-      </c>
+      <c r="A98" s="6"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="10"/>
+      <c r="H98" s="15"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="6"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A99" s="6" t="s">
-        <v>1820</v>
-      </c>
-      <c r="B99" s="10" t="s">
-        <v>1806</v>
-      </c>
-      <c r="C99" s="10" t="s">
-        <v>1821</v>
-      </c>
-      <c r="D99" s="10" t="s">
-        <v>1806</v>
-      </c>
-      <c r="E99" s="6" t="s">
-        <v>1807</v>
-      </c>
-      <c r="F99" s="10">
-        <v>48161</v>
-      </c>
-      <c r="G99" s="10" t="s">
-        <v>1822</v>
-      </c>
-      <c r="H99" s="15" t="s">
-        <v>569</v>
-      </c>
-      <c r="I99" s="6">
-        <v>8192818</v>
-      </c>
-      <c r="J99" s="6" t="s">
-        <v>56</v>
-      </c>
+      <c r="A99" s="6"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="10"/>
+      <c r="H99" s="15"/>
+      <c r="I99" s="6"/>
+      <c r="J99" s="6"/>
     </row>
     <row r="100" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="54" t="s">
-        <v>1828</v>
-      </c>
-      <c r="B100" s="54" t="s">
-        <v>1829</v>
-      </c>
-      <c r="C100" s="54" t="s">
-        <v>1827</v>
-      </c>
-      <c r="D100" s="54" t="s">
-        <v>1829</v>
-      </c>
-      <c r="E100" s="54" t="s">
-        <v>1807</v>
-      </c>
-      <c r="F100" s="54">
-        <v>48909</v>
-      </c>
-      <c r="G100" s="54" t="s">
-        <v>1830</v>
-      </c>
-      <c r="H100" s="42" t="s">
-        <v>569</v>
-      </c>
-      <c r="I100" s="54">
-        <v>897651456</v>
-      </c>
-      <c r="J100" s="54" t="s">
-        <v>56</v>
-      </c>
+      <c r="A100" s="54"/>
+      <c r="B100" s="54"/>
+      <c r="C100" s="54"/>
+      <c r="D100" s="54"/>
+      <c r="E100" s="54"/>
+      <c r="F100" s="54"/>
+      <c r="G100" s="54"/>
+      <c r="H100" s="42"/>
+      <c r="I100" s="54"/>
+      <c r="J100" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11007,7 +10715,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F102" sqref="F102"/>
+      <selection pane="bottomLeft" activeCell="B96" sqref="A96:XFD96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13491,31 +13199,10 @@
         <v>902</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A96" s="10" t="s">
-        <v>1812</v>
-      </c>
-      <c r="B96" s="10" t="s">
-        <v>1817</v>
-      </c>
-      <c r="C96" s="10" t="s">
-        <v>1816</v>
-      </c>
-      <c r="D96" s="10" t="s">
-        <v>1817</v>
-      </c>
-      <c r="E96" s="10" t="s">
-        <v>1818</v>
-      </c>
-      <c r="F96" s="6" t="s">
-        <v>1819</v>
-      </c>
-      <c r="G96" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="H96" s="10" t="s">
-        <v>902</v>
-      </c>
+    <row r="96" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C96" s="10"/>
+      <c r="F96" s="6"/>
+      <c r="H96" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H6"/>
@@ -13589,10 +13276,9 @@
     <hyperlink ref="H95" r:id="rId67" display="http://www.fakephonenumber.org/UnitedStates/phone_number/areacode/410942"/>
     <hyperlink ref="H93" r:id="rId68" display="http://www.fakephonenumber.org/UnitedStates/phone_number/areacode/240784"/>
     <hyperlink ref="H92" r:id="rId69" display="http://www.fakephonenumber.org/UnitedStates/phone_number/areacode/240290"/>
-    <hyperlink ref="H96" r:id="rId70" display="http://www.fakephonenumber.org/UnitedStates/phone_number/areacode/410942"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId71"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId70"/>
 </worksheet>
 </file>
 
@@ -13600,7 +13286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O77"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
@@ -17027,7 +16713,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D106" sqref="D106"/>
+      <selection pane="bottomLeft" activeCell="A97" sqref="A97:XFD100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21564,192 +21250,37 @@
       </c>
     </row>
     <row r="97" spans="1:15" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="54" t="s">
-        <v>1828</v>
-      </c>
-      <c r="B97" s="34" t="s">
-        <v>1809</v>
-      </c>
-      <c r="C97" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="D97" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="E97" s="34" t="s">
-        <v>903</v>
-      </c>
-      <c r="F97" s="53" t="s">
-        <v>1805</v>
-      </c>
-      <c r="G97" s="53" t="s">
-        <v>1806</v>
-      </c>
-      <c r="H97" s="53" t="s">
-        <v>1807</v>
-      </c>
-      <c r="I97" s="53">
-        <v>48161</v>
-      </c>
-      <c r="J97" s="34" t="s">
-        <v>1808</v>
-      </c>
-      <c r="K97" s="34" t="s">
-        <v>1810</v>
-      </c>
-      <c r="L97" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="M97" s="34">
-        <v>6610229539</v>
-      </c>
-      <c r="N97" s="34" t="s">
-        <v>1337</v>
-      </c>
-      <c r="O97" s="34" t="s">
-        <v>1811</v>
-      </c>
+      <c r="A97" s="54"/>
+      <c r="F97" s="53"/>
+      <c r="G97" s="53"/>
+      <c r="H97" s="53"/>
+      <c r="I97" s="53"/>
     </row>
     <row r="98" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="6" t="s">
-        <v>1820</v>
-      </c>
-      <c r="B98" s="10" t="s">
-        <v>1045</v>
-      </c>
-      <c r="C98" s="10" t="s">
-        <v>1823</v>
-      </c>
-      <c r="D98" s="10" t="s">
-        <v>1823</v>
-      </c>
-      <c r="E98" s="6" t="s">
-        <v>1824</v>
-      </c>
-      <c r="F98" s="10" t="s">
-        <v>1821</v>
-      </c>
-      <c r="G98" s="10" t="s">
-        <v>1806</v>
-      </c>
-      <c r="H98" s="6" t="s">
-        <v>1807</v>
-      </c>
-      <c r="I98" s="10">
-        <v>48161</v>
-      </c>
-      <c r="J98" s="6" t="s">
-        <v>1822</v>
-      </c>
-      <c r="K98" s="10" t="s">
-        <v>1825</v>
-      </c>
-      <c r="L98" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="M98" s="34" t="s">
-        <v>1826</v>
-      </c>
-      <c r="N98" s="34" t="s">
-        <v>1336</v>
-      </c>
-      <c r="O98" s="34" t="s">
-        <v>1836</v>
-      </c>
+      <c r="A98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="J98" s="6"/>
+      <c r="L98" s="6"/>
+      <c r="M98" s="34"/>
+      <c r="N98" s="34"/>
+      <c r="O98" s="34"/>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A99" s="40" t="s">
-        <v>1812</v>
-      </c>
-      <c r="B99" s="19" t="s">
-        <v>1832</v>
-      </c>
-      <c r="C99" s="19" t="s">
-        <v>1833</v>
-      </c>
-      <c r="D99" s="19" t="s">
-        <v>1833</v>
-      </c>
-      <c r="E99" s="19" t="s">
-        <v>1834</v>
-      </c>
-      <c r="F99" s="54" t="s">
-        <v>1813</v>
-      </c>
-      <c r="G99" s="54" t="s">
-        <v>1804</v>
-      </c>
-      <c r="H99" s="54" t="s">
-        <v>1427</v>
-      </c>
-      <c r="I99" s="54">
-        <v>43634</v>
-      </c>
-      <c r="J99" s="19" t="s">
-        <v>1831</v>
-      </c>
-      <c r="K99" s="3" t="s">
-        <v>1835</v>
-      </c>
-      <c r="L99" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="M99" s="6">
-        <v>4370286633</v>
-      </c>
-      <c r="N99" s="34" t="s">
-        <v>1336</v>
-      </c>
-      <c r="O99" s="19" t="s">
-        <v>1846</v>
-      </c>
+      <c r="F99" s="54"/>
+      <c r="G99" s="54"/>
+      <c r="H99" s="54"/>
+      <c r="I99" s="54"/>
+      <c r="N99" s="34"/>
     </row>
     <row r="100" spans="1:15" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="54" t="s">
-        <v>1837</v>
-      </c>
-      <c r="B100" s="34" t="s">
-        <v>1841</v>
-      </c>
-      <c r="C100" s="34" t="s">
-        <v>1842</v>
-      </c>
-      <c r="D100" s="34" t="s">
-        <v>1842</v>
-      </c>
-      <c r="E100" s="34" t="s">
-        <v>1843</v>
-      </c>
-      <c r="F100" s="54" t="s">
-        <v>1838</v>
-      </c>
-      <c r="G100" s="54" t="s">
-        <v>1839</v>
-      </c>
-      <c r="H100" s="54" t="s">
-        <v>1807</v>
-      </c>
-      <c r="I100" s="54">
-        <v>48182</v>
-      </c>
-      <c r="J100" s="34" t="s">
-        <v>1840</v>
-      </c>
-      <c r="K100" s="29" t="s">
-        <v>1844</v>
-      </c>
-      <c r="L100" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="M100" s="6">
-        <v>7393971909</v>
-      </c>
-      <c r="N100" s="34" t="s">
-        <v>1336</v>
-      </c>
-      <c r="O100" s="34" t="s">
-        <v>1845</v>
-      </c>
+      <c r="A100" s="54"/>
+      <c r="F100" s="54"/>
+      <c r="G100" s="54"/>
+      <c r="H100" s="54"/>
+      <c r="I100" s="54"/>
+      <c r="K100" s="29"/>
+      <c r="M100" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:O96"/>
@@ -21859,7 +21390,7 @@
   <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23901,7 +23432,7 @@
   <dimension ref="A1:W24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23967,7 +23498,7 @@
         <v>69</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>1847</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -24014,7 +23545,7 @@
         <v>173</v>
       </c>
       <c r="O2" s="58" t="s">
-        <v>1848</v>
+        <v>1805</v>
       </c>
       <c r="P2" s="29"/>
       <c r="Q2" s="29"/>
@@ -24069,7 +23600,7 @@
         <v>175</v>
       </c>
       <c r="O3" s="58" t="s">
-        <v>1849</v>
+        <v>1806</v>
       </c>
       <c r="P3" s="29"/>
       <c r="Q3" s="29"/>
@@ -24124,7 +23655,7 @@
         <v>174</v>
       </c>
       <c r="O4" s="58" t="s">
-        <v>1850</v>
+        <v>1807</v>
       </c>
       <c r="P4" s="29"/>
       <c r="Q4" s="29"/>
@@ -24179,7 +23710,7 @@
         <v>191</v>
       </c>
       <c r="O5" s="58" t="s">
-        <v>1851</v>
+        <v>1808</v>
       </c>
       <c r="P5" s="29"/>
       <c r="Q5" s="29"/>
@@ -24234,7 +23765,7 @@
         <v>192</v>
       </c>
       <c r="O6" s="58" t="s">
-        <v>1852</v>
+        <v>1809</v>
       </c>
       <c r="P6" s="29"/>
       <c r="Q6" s="29"/>
@@ -24289,7 +23820,7 @@
         <v>179</v>
       </c>
       <c r="O7" s="58" t="s">
-        <v>1853</v>
+        <v>1810</v>
       </c>
       <c r="P7" s="29"/>
       <c r="Q7" s="29"/>
@@ -24344,7 +23875,7 @@
         <v>187</v>
       </c>
       <c r="O8" s="58" t="s">
-        <v>1854</v>
+        <v>1811</v>
       </c>
       <c r="P8" s="29"/>
       <c r="Q8" s="29"/>
@@ -24399,7 +23930,7 @@
         <v>188</v>
       </c>
       <c r="O9" s="58" t="s">
-        <v>1855</v>
+        <v>1812</v>
       </c>
       <c r="P9" s="29"/>
       <c r="Q9" s="29"/>
@@ -24454,7 +23985,7 @@
         <v>189</v>
       </c>
       <c r="O10" s="58" t="s">
-        <v>1856</v>
+        <v>1813</v>
       </c>
       <c r="P10" s="29"/>
       <c r="Q10" s="29"/>
@@ -24509,7 +24040,7 @@
         <v>176</v>
       </c>
       <c r="O11" s="58" t="s">
-        <v>1857</v>
+        <v>1814</v>
       </c>
       <c r="P11" s="29"/>
       <c r="Q11" s="29"/>
@@ -24564,7 +24095,7 @@
         <v>177</v>
       </c>
       <c r="O12" s="58" t="s">
-        <v>1858</v>
+        <v>1815</v>
       </c>
       <c r="P12" s="29"/>
       <c r="Q12" s="29"/>
@@ -24619,7 +24150,7 @@
         <v>190</v>
       </c>
       <c r="O13" s="58" t="s">
-        <v>1859</v>
+        <v>1816</v>
       </c>
       <c r="P13" s="29"/>
       <c r="Q13" s="29"/>

</xml_diff>

<commit_message>
combine conf data in the main file
20941 - Update Demo site with Latest code and Test Data
</commit_message>
<xml_diff>
--- a/src/main/resources/OCP.xlsx
+++ b/src/main/resources/OCP.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\c2s-ws\ocp-ws\ocp-test-data\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\intellij-workspaces\ocp\ocp-test-data\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8892" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8892" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Organizations" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4350" uniqueCount="1817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4472" uniqueCount="1860">
   <si>
     <t>First Name</t>
   </si>
@@ -5463,6 +5463,135 @@
   </si>
   <si>
     <t>johnny.jesus@mailinator.com</t>
+  </si>
+  <si>
+    <t>Toledo</t>
+  </si>
+  <si>
+    <t>903 S. Telegraph, Ste. A</t>
+  </si>
+  <si>
+    <t>Monroe</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>734-555-7200</t>
+  </si>
+  <si>
+    <t>Ellen</t>
+  </si>
+  <si>
+    <t>ellen.davis@mailinator.com</t>
+  </si>
+  <si>
+    <t>e.davis.cc</t>
+  </si>
+  <si>
+    <t>Substance Abuse Services, Inc</t>
+  </si>
+  <si>
+    <t>1916 N 12th St</t>
+  </si>
+  <si>
+    <t>SAS0001</t>
+  </si>
+  <si>
+    <t>Toledo Location</t>
+  </si>
+  <si>
+    <t>Methadone Maintenance Treatment Program (MMTP)</t>
+  </si>
+  <si>
+    <t>RESIDENTIAL SUB-ACUTE DETOXIFICATION (detox)</t>
+  </si>
+  <si>
+    <t>Drug and/or Alcohol Counselling</t>
+  </si>
+  <si>
+    <t>Rehabilitation</t>
+  </si>
+  <si>
+    <t>Monroe County Probation</t>
+  </si>
+  <si>
+    <t>125 E 2nd St</t>
+  </si>
+  <si>
+    <t>734-555-7100</t>
+  </si>
+  <si>
+    <t>Reagan</t>
+  </si>
+  <si>
+    <t>Probation Officer</t>
+  </si>
+  <si>
+    <t>daniel.reagan@mailenator.com</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>333 S. Grand Ave P.O. Box 30195</t>
+  </si>
+  <si>
+    <t>Michigan Department of Health and Human Services</t>
+  </si>
+  <si>
+    <t>Lansing</t>
+  </si>
+  <si>
+    <t>517-335-9030</t>
+  </si>
+  <si>
+    <t>419-555-6020</t>
+  </si>
+  <si>
+    <t>Jordon</t>
+  </si>
+  <si>
+    <t>Emmett</t>
+  </si>
+  <si>
+    <t>Addiction Psychiatry</t>
+  </si>
+  <si>
+    <t>jordon.emmett@mailenator.com</t>
+  </si>
+  <si>
+    <t>d.reagan.cm</t>
+  </si>
+  <si>
+    <t>Bay Creek Emergency Services</t>
+  </si>
+  <si>
+    <t>7157 Jackman Rd</t>
+  </si>
+  <si>
+    <t>Temperance</t>
+  </si>
+  <si>
+    <t>734-555-9779</t>
+  </si>
+  <si>
+    <t>Trace</t>
+  </si>
+  <si>
+    <t>Farooq</t>
+  </si>
+  <si>
+    <t>Emergency Medicine Physician</t>
+  </si>
+  <si>
+    <t>trace.farooq@mailenator.com</t>
+  </si>
+  <si>
+    <t>t.farooq.cm</t>
+  </si>
+  <si>
+    <t>j.emmett.cm</t>
   </si>
   <si>
     <t>Contact-Email</t>
@@ -5507,7 +5636,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="00000"/>
@@ -6921,7 +7050,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD33"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7516,41 +7645,120 @@
       </c>
     </row>
     <row r="21" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
+      <c r="A21" s="54" t="s">
+        <v>1837</v>
+      </c>
+      <c r="B21" s="56" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C21" s="56" t="s">
+        <v>1838</v>
+      </c>
+      <c r="D21" s="56" t="s">
+        <v>1839</v>
+      </c>
+      <c r="E21" s="56" t="s">
+        <v>1807</v>
+      </c>
+      <c r="F21" s="56">
+        <v>48182</v>
+      </c>
+      <c r="G21" s="42" t="s">
+        <v>1840</v>
+      </c>
+      <c r="H21" s="54">
+        <v>237645898</v>
+      </c>
+      <c r="I21" s="54" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="22" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
+      <c r="A22" s="54" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B22" s="54" t="s">
+        <v>1829</v>
+      </c>
+      <c r="C22" s="54" t="s">
+        <v>1827</v>
+      </c>
+      <c r="D22" s="54" t="s">
+        <v>1829</v>
+      </c>
+      <c r="E22" s="54" t="s">
+        <v>1807</v>
+      </c>
+      <c r="F22" s="54">
+        <v>48909</v>
+      </c>
+      <c r="G22" s="54" t="s">
+        <v>1830</v>
+      </c>
+      <c r="H22" s="54">
+        <v>897651456</v>
+      </c>
+      <c r="I22" s="54" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="23" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="54"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
+      <c r="A23" s="54" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B23" s="54" t="s">
+        <v>1815</v>
+      </c>
+      <c r="C23" s="54" t="s">
+        <v>1813</v>
+      </c>
+      <c r="D23" s="54" t="s">
+        <v>1804</v>
+      </c>
+      <c r="E23" s="54" t="s">
+        <v>1427</v>
+      </c>
+      <c r="F23" s="54">
+        <v>43634</v>
+      </c>
+      <c r="G23" s="54" t="s">
+        <v>1831</v>
+      </c>
+      <c r="H23" s="54">
+        <v>987122345</v>
+      </c>
+      <c r="I23" s="54" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="A24" s="10" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>1806</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>1821</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>1806</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>1807</v>
+      </c>
+      <c r="F24" s="10">
+        <v>48161</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>1822</v>
+      </c>
+      <c r="H24" s="10">
+        <v>8192818</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7565,8 +7773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97:XFD107"/>
+    <sheetView topLeftCell="A76" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10657,48 +10865,132 @@
       </c>
     </row>
     <row r="97" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="54"/>
-      <c r="B97" s="56"/>
-      <c r="C97" s="56"/>
-      <c r="D97" s="56"/>
-      <c r="E97" s="56"/>
-      <c r="F97" s="56"/>
-      <c r="G97" s="42"/>
-      <c r="H97" s="15"/>
-      <c r="I97" s="54"/>
-      <c r="J97" s="54"/>
+      <c r="A97" s="54" t="s">
+        <v>1837</v>
+      </c>
+      <c r="B97" s="56" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C97" s="56" t="s">
+        <v>1838</v>
+      </c>
+      <c r="D97" s="56" t="s">
+        <v>1839</v>
+      </c>
+      <c r="E97" s="56" t="s">
+        <v>1807</v>
+      </c>
+      <c r="F97" s="56">
+        <v>48182</v>
+      </c>
+      <c r="G97" s="42" t="s">
+        <v>1840</v>
+      </c>
+      <c r="H97" s="15" t="s">
+        <v>569</v>
+      </c>
+      <c r="I97" s="54">
+        <v>237645898</v>
+      </c>
+      <c r="J97" s="54" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A98" s="6"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="10"/>
-      <c r="E98" s="6"/>
-      <c r="F98" s="10"/>
-      <c r="H98" s="15"/>
-      <c r="I98" s="6"/>
-      <c r="J98" s="6"/>
+      <c r="A98" s="6" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B98" s="10" t="s">
+        <v>1815</v>
+      </c>
+      <c r="C98" s="10" t="s">
+        <v>1813</v>
+      </c>
+      <c r="D98" s="10" t="s">
+        <v>1804</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>1427</v>
+      </c>
+      <c r="F98" s="10">
+        <v>43634</v>
+      </c>
+      <c r="G98" s="10" t="s">
+        <v>1808</v>
+      </c>
+      <c r="H98" s="15" t="s">
+        <v>569</v>
+      </c>
+      <c r="I98" s="6" t="s">
+        <v>1814</v>
+      </c>
+      <c r="J98" s="6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A99" s="6"/>
-      <c r="C99" s="10"/>
-      <c r="D99" s="10"/>
-      <c r="E99" s="6"/>
-      <c r="F99" s="10"/>
-      <c r="H99" s="15"/>
-      <c r="I99" s="6"/>
-      <c r="J99" s="6"/>
+      <c r="A99" s="6" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B99" s="10" t="s">
+        <v>1806</v>
+      </c>
+      <c r="C99" s="10" t="s">
+        <v>1821</v>
+      </c>
+      <c r="D99" s="10" t="s">
+        <v>1806</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>1807</v>
+      </c>
+      <c r="F99" s="10">
+        <v>48161</v>
+      </c>
+      <c r="G99" s="10" t="s">
+        <v>1822</v>
+      </c>
+      <c r="H99" s="15" t="s">
+        <v>569</v>
+      </c>
+      <c r="I99" s="6">
+        <v>8192818</v>
+      </c>
+      <c r="J99" s="6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="100" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="54"/>
-      <c r="B100" s="54"/>
-      <c r="C100" s="54"/>
-      <c r="D100" s="54"/>
-      <c r="E100" s="54"/>
-      <c r="F100" s="54"/>
-      <c r="G100" s="54"/>
-      <c r="H100" s="42"/>
-      <c r="I100" s="54"/>
-      <c r="J100" s="54"/>
+      <c r="A100" s="54" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B100" s="54" t="s">
+        <v>1829</v>
+      </c>
+      <c r="C100" s="54" t="s">
+        <v>1827</v>
+      </c>
+      <c r="D100" s="54" t="s">
+        <v>1829</v>
+      </c>
+      <c r="E100" s="54" t="s">
+        <v>1807</v>
+      </c>
+      <c r="F100" s="54">
+        <v>48909</v>
+      </c>
+      <c r="G100" s="54" t="s">
+        <v>1830</v>
+      </c>
+      <c r="H100" s="42" t="s">
+        <v>569</v>
+      </c>
+      <c r="I100" s="54">
+        <v>897651456</v>
+      </c>
+      <c r="J100" s="54" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10715,7 +11007,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B96" sqref="A96:XFD96"/>
+      <selection pane="bottomLeft" activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13199,10 +13491,31 @@
         <v>902</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C96" s="10"/>
-      <c r="F96" s="6"/>
-      <c r="H96" s="10"/>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A96" s="10" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>1817</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>1816</v>
+      </c>
+      <c r="D96" s="10" t="s">
+        <v>1817</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>1818</v>
+      </c>
+      <c r="F96" s="6" t="s">
+        <v>1819</v>
+      </c>
+      <c r="G96" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="H96" s="10" t="s">
+        <v>902</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H6"/>
@@ -13276,9 +13589,10 @@
     <hyperlink ref="H95" r:id="rId67" display="http://www.fakephonenumber.org/UnitedStates/phone_number/areacode/410942"/>
     <hyperlink ref="H93" r:id="rId68" display="http://www.fakephonenumber.org/UnitedStates/phone_number/areacode/240784"/>
     <hyperlink ref="H92" r:id="rId69" display="http://www.fakephonenumber.org/UnitedStates/phone_number/areacode/240290"/>
+    <hyperlink ref="H96" r:id="rId70" display="http://www.fakephonenumber.org/UnitedStates/phone_number/areacode/410942"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId70"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId71"/>
 </worksheet>
 </file>
 
@@ -13286,7 +13600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O77"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
@@ -16713,7 +17027,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A97" sqref="A97:XFD100"/>
+      <selection pane="bottomLeft" activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21250,37 +21564,192 @@
       </c>
     </row>
     <row r="97" spans="1:15" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="54"/>
-      <c r="F97" s="53"/>
-      <c r="G97" s="53"/>
-      <c r="H97" s="53"/>
-      <c r="I97" s="53"/>
+      <c r="A97" s="54" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B97" s="34" t="s">
+        <v>1809</v>
+      </c>
+      <c r="C97" s="34" t="s">
+        <v>475</v>
+      </c>
+      <c r="D97" s="34" t="s">
+        <v>475</v>
+      </c>
+      <c r="E97" s="34" t="s">
+        <v>903</v>
+      </c>
+      <c r="F97" s="53" t="s">
+        <v>1805</v>
+      </c>
+      <c r="G97" s="53" t="s">
+        <v>1806</v>
+      </c>
+      <c r="H97" s="53" t="s">
+        <v>1807</v>
+      </c>
+      <c r="I97" s="53">
+        <v>48161</v>
+      </c>
+      <c r="J97" s="34" t="s">
+        <v>1808</v>
+      </c>
+      <c r="K97" s="34" t="s">
+        <v>1810</v>
+      </c>
+      <c r="L97" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="M97" s="34">
+        <v>6610229539</v>
+      </c>
+      <c r="N97" s="34" t="s">
+        <v>1337</v>
+      </c>
+      <c r="O97" s="34" t="s">
+        <v>1811</v>
+      </c>
     </row>
     <row r="98" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="6"/>
-      <c r="E98" s="6"/>
-      <c r="H98" s="6"/>
-      <c r="J98" s="6"/>
-      <c r="L98" s="6"/>
-      <c r="M98" s="34"/>
-      <c r="N98" s="34"/>
-      <c r="O98" s="34"/>
+      <c r="A98" s="6" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B98" s="10" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C98" s="10" t="s">
+        <v>1823</v>
+      </c>
+      <c r="D98" s="10" t="s">
+        <v>1823</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>1824</v>
+      </c>
+      <c r="F98" s="10" t="s">
+        <v>1821</v>
+      </c>
+      <c r="G98" s="10" t="s">
+        <v>1806</v>
+      </c>
+      <c r="H98" s="6" t="s">
+        <v>1807</v>
+      </c>
+      <c r="I98" s="10">
+        <v>48161</v>
+      </c>
+      <c r="J98" s="6" t="s">
+        <v>1822</v>
+      </c>
+      <c r="K98" s="10" t="s">
+        <v>1825</v>
+      </c>
+      <c r="L98" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M98" s="34" t="s">
+        <v>1826</v>
+      </c>
+      <c r="N98" s="34" t="s">
+        <v>1336</v>
+      </c>
+      <c r="O98" s="34" t="s">
+        <v>1836</v>
+      </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F99" s="54"/>
-      <c r="G99" s="54"/>
-      <c r="H99" s="54"/>
-      <c r="I99" s="54"/>
-      <c r="N99" s="34"/>
+      <c r="A99" s="40" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B99" s="19" t="s">
+        <v>1832</v>
+      </c>
+      <c r="C99" s="19" t="s">
+        <v>1833</v>
+      </c>
+      <c r="D99" s="19" t="s">
+        <v>1833</v>
+      </c>
+      <c r="E99" s="19" t="s">
+        <v>1834</v>
+      </c>
+      <c r="F99" s="54" t="s">
+        <v>1813</v>
+      </c>
+      <c r="G99" s="54" t="s">
+        <v>1804</v>
+      </c>
+      <c r="H99" s="54" t="s">
+        <v>1427</v>
+      </c>
+      <c r="I99" s="54">
+        <v>43634</v>
+      </c>
+      <c r="J99" s="19" t="s">
+        <v>1831</v>
+      </c>
+      <c r="K99" s="3" t="s">
+        <v>1835</v>
+      </c>
+      <c r="L99" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M99" s="6">
+        <v>4370286633</v>
+      </c>
+      <c r="N99" s="34" t="s">
+        <v>1336</v>
+      </c>
+      <c r="O99" s="19" t="s">
+        <v>1846</v>
+      </c>
     </row>
     <row r="100" spans="1:15" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="54"/>
-      <c r="F100" s="54"/>
-      <c r="G100" s="54"/>
-      <c r="H100" s="54"/>
-      <c r="I100" s="54"/>
-      <c r="K100" s="29"/>
-      <c r="M100" s="6"/>
+      <c r="A100" s="54" t="s">
+        <v>1837</v>
+      </c>
+      <c r="B100" s="34" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C100" s="34" t="s">
+        <v>1842</v>
+      </c>
+      <c r="D100" s="34" t="s">
+        <v>1842</v>
+      </c>
+      <c r="E100" s="34" t="s">
+        <v>1843</v>
+      </c>
+      <c r="F100" s="54" t="s">
+        <v>1838</v>
+      </c>
+      <c r="G100" s="54" t="s">
+        <v>1839</v>
+      </c>
+      <c r="H100" s="54" t="s">
+        <v>1807</v>
+      </c>
+      <c r="I100" s="54">
+        <v>48182</v>
+      </c>
+      <c r="J100" s="34" t="s">
+        <v>1840</v>
+      </c>
+      <c r="K100" s="29" t="s">
+        <v>1844</v>
+      </c>
+      <c r="L100" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="M100" s="6">
+        <v>7393971909</v>
+      </c>
+      <c r="N100" s="34" t="s">
+        <v>1336</v>
+      </c>
+      <c r="O100" s="34" t="s">
+        <v>1845</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:O96"/>
@@ -21390,7 +21859,7 @@
   <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23432,7 +23901,7 @@
   <dimension ref="A1:W24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23498,7 +23967,7 @@
         <v>69</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>1804</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -23545,7 +24014,7 @@
         <v>173</v>
       </c>
       <c r="O2" s="58" t="s">
-        <v>1805</v>
+        <v>1848</v>
       </c>
       <c r="P2" s="29"/>
       <c r="Q2" s="29"/>
@@ -23600,7 +24069,7 @@
         <v>175</v>
       </c>
       <c r="O3" s="58" t="s">
-        <v>1806</v>
+        <v>1849</v>
       </c>
       <c r="P3" s="29"/>
       <c r="Q3" s="29"/>
@@ -23655,7 +24124,7 @@
         <v>174</v>
       </c>
       <c r="O4" s="58" t="s">
-        <v>1807</v>
+        <v>1850</v>
       </c>
       <c r="P4" s="29"/>
       <c r="Q4" s="29"/>
@@ -23710,7 +24179,7 @@
         <v>191</v>
       </c>
       <c r="O5" s="58" t="s">
-        <v>1808</v>
+        <v>1851</v>
       </c>
       <c r="P5" s="29"/>
       <c r="Q5" s="29"/>
@@ -23765,7 +24234,7 @@
         <v>192</v>
       </c>
       <c r="O6" s="58" t="s">
-        <v>1809</v>
+        <v>1852</v>
       </c>
       <c r="P6" s="29"/>
       <c r="Q6" s="29"/>
@@ -23820,7 +24289,7 @@
         <v>179</v>
       </c>
       <c r="O7" s="58" t="s">
-        <v>1810</v>
+        <v>1853</v>
       </c>
       <c r="P7" s="29"/>
       <c r="Q7" s="29"/>
@@ -23875,7 +24344,7 @@
         <v>187</v>
       </c>
       <c r="O8" s="58" t="s">
-        <v>1811</v>
+        <v>1854</v>
       </c>
       <c r="P8" s="29"/>
       <c r="Q8" s="29"/>
@@ -23930,7 +24399,7 @@
         <v>188</v>
       </c>
       <c r="O9" s="58" t="s">
-        <v>1812</v>
+        <v>1855</v>
       </c>
       <c r="P9" s="29"/>
       <c r="Q9" s="29"/>
@@ -23985,7 +24454,7 @@
         <v>189</v>
       </c>
       <c r="O10" s="58" t="s">
-        <v>1813</v>
+        <v>1856</v>
       </c>
       <c r="P10" s="29"/>
       <c r="Q10" s="29"/>
@@ -24040,7 +24509,7 @@
         <v>176</v>
       </c>
       <c r="O11" s="58" t="s">
-        <v>1814</v>
+        <v>1857</v>
       </c>
       <c r="P11" s="29"/>
       <c r="Q11" s="29"/>
@@ -24095,7 +24564,7 @@
         <v>177</v>
       </c>
       <c r="O12" s="58" t="s">
-        <v>1815</v>
+        <v>1858</v>
       </c>
       <c r="P12" s="29"/>
       <c r="Q12" s="29"/>
@@ -24150,7 +24619,7 @@
         <v>190</v>
       </c>
       <c r="O13" s="58" t="s">
-        <v>1816</v>
+        <v>1859</v>
       </c>
       <c r="P13" s="29"/>
       <c r="Q13" s="29"/>

</xml_diff>